<commit_message>
QAQC updates, changes to nd vs missing values, copies per liter update
</commit_message>
<xml_diff>
--- a/qpcr_analyzer/qpcr_template_ottawa.xlsx
+++ b/qpcr_analyzer/qpcr_template_ottawa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinwellman/Documents/Health/Wastewater/Code/odm-qpcr-analyzer/qpcr_analyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC24C726-604E-964D-929E-8FACA9C54E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B4EFD3-4DA2-CB45-A8CF-2543F50DB6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{9359BC57-A822-3445-B588-7E071C6D13C9}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="108">
   <si>
     <t>qPCR Data</t>
   </si>
@@ -169,9 +169,6 @@
 STDEV</t>
   </si>
   <si>
-    <t>2^Ct</t>
-  </si>
-  <si>
     <t>STDEV</t>
   </si>
   <si>
@@ -257,54 +254,6 @@
   </si>
   <si>
     <t>{siteID}</t>
-  </si>
-  <si>
-    <t>{value_npmmov_dil10_0|}</t>
-  </si>
-  <si>
-    <t>{value_npmmov_dil10_1|}</t>
-  </si>
-  <si>
-    <t>{value_npmmov_dil10_2|}</t>
-  </si>
-  <si>
-    <t>{value_npmmov_dil40_0|}</t>
-  </si>
-  <si>
-    <t>{value_npmmov_dil40_1|}</t>
-  </si>
-  <si>
-    <t>{value_npmmov_dil40_2|}</t>
-  </si>
-  <si>
-    <t>{value_npmmov_0|}</t>
-  </si>
-  <si>
-    <t>{value_npmmov_1|}</t>
-  </si>
-  <si>
-    <t>{value_npmmov_2|}</t>
-  </si>
-  <si>
-    <t>{value_0|}</t>
-  </si>
-  <si>
-    <t>{value_1|}</t>
-  </si>
-  <si>
-    <t>{value_2|}</t>
-  </si>
-  <si>
-    <t>{value_emptytubemass_0|}</t>
-  </si>
-  <si>
-    <t>{value_tottubemass_0|}</t>
-  </si>
-  <si>
-    <t>{value_setsol_0|}</t>
-  </si>
-  <si>
-    <t>{value_extmass_0|}</t>
   </si>
   <si>
     <t>nPMMoV Ct</t>
@@ -329,22 +278,6 @@
 STDEV</t>
   </si>
   <si>
-    <t>Copies per Copies of nPMMoV
-AVG</t>
-  </si>
-  <si>
-    <t>Copies per Copies of nPMMoV * 10^3
-AVG</t>
-  </si>
-  <si>
-    <t>Copies per Copies of nPMMoV
-STDEV</t>
-  </si>
-  <si>
-    <t>Copies per Copies of nPMMoV * 10^3
-STDEV</t>
-  </si>
-  <si>
     <t>Copies per Copies of nPMMoV</t>
   </si>
   <si>
@@ -369,6 +302,66 @@
   <si>
     <t>ΔCt
 1/40 - Full</t>
+  </si>
+  <si>
+    <t>{value_0|&lt;ND&gt;|&lt;MISSING&gt;}</t>
+  </si>
+  <si>
+    <t>{value_1|&lt;ND&gt;|&lt;MISSING&gt;}</t>
+  </si>
+  <si>
+    <t>{value_2|&lt;ND&gt;|&lt;MISSING&gt;}</t>
+  </si>
+  <si>
+    <t>{value_npmmov_dil10_0|&lt;ND&gt;|&lt;MISSING&gt;}</t>
+  </si>
+  <si>
+    <t>{value_npmmov_dil10_1|&lt;ND&gt;|&lt;MISSING&gt;}</t>
+  </si>
+  <si>
+    <t>{value_npmmov_dil10_2|&lt;ND&gt;|&lt;MISSING&gt;}</t>
+  </si>
+  <si>
+    <t>Total volume (mL)</t>
+  </si>
+  <si>
+    <t>{value_npmmov_dil40_0|&lt;ND&gt;|&lt;MISSING&gt;}</t>
+  </si>
+  <si>
+    <t>{value_npmmov_dil40_1|&lt;ND&gt;|&lt;MISSING&gt;}</t>
+  </si>
+  <si>
+    <t>{value_npmmov_dil40_2|&lt;ND&gt;|&lt;MISSING&gt;}</t>
+  </si>
+  <si>
+    <t>{value_npmmov_0|&lt;ND&gt;|&lt;MISSING&gt;}</t>
+  </si>
+  <si>
+    <t>{value_npmmov_1|&lt;ND&gt;|&lt;MISSING&gt;}</t>
+  </si>
+  <si>
+    <t>{value_npmmov_2|&lt;ND&gt;|&lt;MISSING&gt;}</t>
+  </si>
+  <si>
+    <t>{value_totvol_0||}</t>
+  </si>
+  <si>
+    <t>{value_emptytubemass_0||}</t>
+  </si>
+  <si>
+    <t>{value_tottubemass_0||}</t>
+  </si>
+  <si>
+    <t>{value_setsol_0||}</t>
+  </si>
+  <si>
+    <t>{value_extmass_0||}</t>
+  </si>
+  <si>
+    <t>main_col_inhibition_10_nodil_dct</t>
+  </si>
+  <si>
+    <t>main_col_inhibition_40_nodil_dct</t>
   </si>
 </sst>
 </file>
@@ -1392,10 +1385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A78BE4-03D0-4C45-A8C6-85FB2F5005D2}">
-  <dimension ref="A1:BW10"/>
+  <dimension ref="A1:BS10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AM7" sqref="AM7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1405,141 +1398,151 @@
     <col min="3" max="3" width="14.83203125" customWidth="1"/>
     <col min="4" max="4" width="30.1640625" customWidth="1"/>
     <col min="5" max="6" width="11" customWidth="1"/>
-    <col min="7" max="24" width="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11" customWidth="1"/>
-    <col min="26" max="27" width="16.1640625" customWidth="1"/>
-    <col min="28" max="33" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="21" width="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11" customWidth="1"/>
+    <col min="23" max="25" width="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11" customWidth="1"/>
+    <col min="27" max="28" width="16.1640625" customWidth="1"/>
+    <col min="29" max="33" width="11" bestFit="1" customWidth="1"/>
     <col min="34" max="36" width="15" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="13" customWidth="1"/>
-    <col min="39" max="40" width="11" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.6640625" customWidth="1"/>
-    <col min="45" max="49" width="11" bestFit="1" customWidth="1"/>
-    <col min="50" max="52" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="13" customWidth="1"/>
-    <col min="54" max="55" width="16.1640625" customWidth="1"/>
-    <col min="56" max="56" width="15.33203125" customWidth="1"/>
-    <col min="57" max="57" width="14.1640625" customWidth="1"/>
-    <col min="58" max="58" width="19.6640625" customWidth="1"/>
-    <col min="59" max="59" width="19.33203125" customWidth="1"/>
-    <col min="60" max="60" width="11" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="29.1640625" customWidth="1"/>
-    <col min="62" max="65" width="11" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.6640625" customWidth="1"/>
+    <col min="41" max="45" width="11" bestFit="1" customWidth="1"/>
+    <col min="46" max="48" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="13" customWidth="1"/>
+    <col min="50" max="51" width="16.1640625" customWidth="1"/>
+    <col min="52" max="52" width="15.33203125" customWidth="1"/>
+    <col min="53" max="53" width="14.1640625" customWidth="1"/>
+    <col min="54" max="54" width="19.6640625" customWidth="1"/>
+    <col min="55" max="55" width="19.33203125" customWidth="1"/>
+    <col min="56" max="56" width="11" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="29.1640625" customWidth="1"/>
+    <col min="58" max="61" width="11" bestFit="1" customWidth="1"/>
+    <col min="65" max="67" width="11" bestFit="1" customWidth="1"/>
     <col min="69" max="71" width="11" bestFit="1" customWidth="1"/>
-    <col min="73" max="75" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:71" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>53</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="R1" t="s">
         <v>51</v>
       </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
         <v>51</v>
       </c>
-      <c r="O1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>52</v>
-      </c>
-      <c r="R1" t="s">
-        <v>52</v>
-      </c>
-      <c r="S1" t="s">
-        <v>52</v>
-      </c>
       <c r="T1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="AC1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AD1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AE1" t="s">
         <v>55</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AF1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AX1" t="s">
         <v>58</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AY1" t="s">
         <v>58</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AZ1" t="s">
         <v>58</v>
       </c>
-      <c r="AV1" t="s">
-        <v>57</v>
-      </c>
-      <c r="BB1" t="s">
+      <c r="BA1" t="s">
         <v>59</v>
       </c>
-      <c r="BC1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>60</v>
       </c>
+      <c r="BG1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>61</v>
+      </c>
       <c r="BJ1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="BK1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="BL1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="BM1" t="s">
         <v>62</v>
       </c>
       <c r="BN1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BQ1" t="s">
         <v>64</v>
       </c>
-      <c r="BO1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>63</v>
-      </c>
       <c r="BR1" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="BS1" t="s">
-        <v>66</v>
-      </c>
-      <c r="BT1" s="26"/>
-      <c r="BU1" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:75" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:71" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
@@ -1597,11 +1600,11 @@
       <c r="BA2" s="1"/>
       <c r="BB2" s="1"/>
       <c r="BC2" s="1"/>
-      <c r="BD2" s="1"/>
-      <c r="BE2" s="1"/>
-      <c r="BF2" s="1"/>
-      <c r="BG2" s="1"/>
-      <c r="BH2" s="2"/>
+      <c r="BD2" s="2"/>
+      <c r="BE2" s="3"/>
+      <c r="BF2" s="3"/>
+      <c r="BG2" s="3"/>
+      <c r="BH2" s="3"/>
       <c r="BI2" s="3"/>
       <c r="BJ2" s="3"/>
       <c r="BK2" s="3"/>
@@ -1612,18 +1615,14 @@
       <c r="BP2" s="3"/>
       <c r="BQ2" s="3"/>
       <c r="BR2" s="3"/>
-      <c r="BS2" s="3"/>
-      <c r="BT2" s="3"/>
-      <c r="BU2" s="3"/>
-      <c r="BV2" s="3"/>
-      <c r="BW2" s="4"/>
+      <c r="BS2" s="4"/>
     </row>
-    <row r="3" spans="1:75" s="5" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:71" s="5" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>0</v>
@@ -1642,26 +1641,30 @@
       </c>
       <c r="J3" s="65"/>
       <c r="K3" s="65"/>
-      <c r="AS3" s="53" t="s">
+      <c r="AO3" s="53" t="s">
         <v>1</v>
       </c>
+      <c r="AP3" s="54"/>
+      <c r="AQ3" s="54"/>
+      <c r="AR3" s="54"/>
+      <c r="AS3" s="54"/>
       <c r="AT3" s="54"/>
       <c r="AU3" s="54"/>
       <c r="AV3" s="54"/>
       <c r="AW3" s="54"/>
       <c r="AX3" s="54"/>
       <c r="AY3" s="54"/>
-      <c r="AZ3" s="54"/>
-      <c r="BA3" s="54"/>
-      <c r="BB3" s="54"/>
-      <c r="BC3" s="54"/>
-      <c r="BD3" s="55"/>
-      <c r="BE3" s="28"/>
-      <c r="BF3" s="29"/>
-      <c r="BG3" s="30"/>
-      <c r="BH3" s="56" t="s">
+      <c r="AZ3" s="55"/>
+      <c r="BA3" s="28"/>
+      <c r="BB3" s="29"/>
+      <c r="BC3" s="30"/>
+      <c r="BD3" s="56" t="s">
         <v>2</v>
       </c>
+      <c r="BE3" s="56"/>
+      <c r="BF3" s="56"/>
+      <c r="BG3" s="56"/>
+      <c r="BH3" s="56"/>
       <c r="BI3" s="56"/>
       <c r="BJ3" s="56"/>
       <c r="BK3" s="56"/>
@@ -1672,13 +1675,9 @@
       <c r="BP3" s="56"/>
       <c r="BQ3" s="56"/>
       <c r="BR3" s="56"/>
-      <c r="BS3" s="56"/>
-      <c r="BT3" s="56"/>
-      <c r="BU3" s="56"/>
-      <c r="BV3" s="56"/>
-      <c r="BW3" s="57"/>
+      <c r="BS3" s="57"/>
     </row>
-    <row r="4" spans="1:75" s="5" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:71" s="5" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1692,7 +1691,7 @@
         <v>40</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" s="58" t="s">
         <v>5</v>
@@ -1717,160 +1716,148 @@
         <v>37</v>
       </c>
       <c r="Q4" s="58" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="R4" s="59"/>
       <c r="S4" s="60"/>
       <c r="T4" s="8" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="V4" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="W4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="W4" s="7" t="s">
+      <c r="X4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="X4" s="7" t="s">
+      <c r="Y4" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="Y4" s="7" t="s">
+      <c r="Z4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB4" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="Z4" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA4" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB4" s="61" t="s">
+      <c r="AC4" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="AC4" s="62"/>
-      <c r="AD4" s="63"/>
-      <c r="AE4" s="9" t="s">
+      <c r="AD4" s="62"/>
+      <c r="AE4" s="63"/>
+      <c r="AF4" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="AF4" s="7" t="s">
+      <c r="AG4" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AG4" s="7" t="s">
-        <v>45</v>
-      </c>
       <c r="AH4" s="61" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="AI4" s="62"/>
       <c r="AJ4" s="63"/>
       <c r="AK4" s="7" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="AL4" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="AM4" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="AN4" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="AO4" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="AP4" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="AQ4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="AR4" s="6" t="s">
+      <c r="AN4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AS4" s="61" t="s">
-        <v>101</v>
-      </c>
-      <c r="AT4" s="62"/>
-      <c r="AU4" s="63"/>
-      <c r="AV4" s="18" t="s">
+      <c r="AO4" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP4" s="62"/>
+      <c r="AQ4" s="63"/>
+      <c r="AR4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="AW4" s="18" t="s">
+      <c r="AS4" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT4" s="61" t="s">
         <v>46</v>
       </c>
+      <c r="AU4" s="62"/>
+      <c r="AV4" s="63"/>
+      <c r="AW4" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="AX4" s="61" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="AY4" s="62"/>
       <c r="AZ4" s="63"/>
-      <c r="BA4" s="7" t="s">
+      <c r="BA4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="BB4" s="61" t="s">
-        <v>11</v>
-      </c>
-      <c r="BC4" s="62"/>
-      <c r="BD4" s="63"/>
-      <c r="BE4" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="BF4" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="BG4" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="BH4" s="20" t="s">
+      <c r="BB4" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="BC4" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="BD4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="BI4" s="12" t="s">
+      <c r="BE4" s="12" t="s">
         <v>12</v>
       </c>
+      <c r="BF4" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="BG4" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="BH4" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="BI4" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="BJ4" s="12" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="BK4" s="12" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="BL4" s="12" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="BM4" s="13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BN4" s="12" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="BO4" s="12" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="BP4" s="12" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="BQ4" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="BR4" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="BS4" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="BT4" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="BU4" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="BV4" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="BW4" s="14" t="s">
-        <v>108</v>
+        <v>86</v>
+      </c>
+      <c r="BS4" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:75" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:71" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1884,16 +1871,16 @@
         <v>23</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="J5" s="16" t="e">
         <f>AVERAGE(G5:I5)</f>
@@ -1924,13 +1911,13 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q5" s="16" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="R5" s="16" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="S5" s="16" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="T5" s="16" t="e">
         <f>AVERAGE(Q5:S5)</f>
@@ -1941,47 +1928,46 @@
         <v>#DIV/0!</v>
       </c>
       <c r="V5" s="17" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="W5" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="X5" s="17" t="e">
-        <f>IF(AND(W5&lt;&gt;"",V5&lt;&gt;""),W5-V5,"")</f>
+        <v>102</v>
+      </c>
+      <c r="X5" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y5" s="17" t="e">
+        <f>IF(AND(X5&lt;&gt;"",W5&lt;&gt;""),X5-W5,"")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Y5" s="17" t="s">
-        <v>89</v>
-      </c>
       <c r="Z5" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA5" s="49">
+        <v>104</v>
+      </c>
+      <c r="AA5" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB5" s="49">
         <f>IF(ISERROR(DATEVALUE(B5)),3,IF(DATEVALUE(B5)&gt;=DATE(2021,6,8),3,1.5))</f>
         <v>3</v>
       </c>
-      <c r="AB5" s="17" t="str">
-        <f>IF(L5&lt;&gt;"",(L5/$AA5*100)/$Z5,"")</f>
+      <c r="AC5" s="17" t="str">
+        <f>IF(L5&lt;&gt;"",(L5/$AB5*100)/$AA5,"")</f>
         <v/>
       </c>
-      <c r="AC5" s="17" t="str">
-        <f>IF(M5&lt;&gt;"",(M5/$AA5*100)/$Z5,"")</f>
+      <c r="AD5" s="17" t="str">
+        <f>IF(M5&lt;&gt;"",(M5/$AB5*100)/$AA5,"")</f>
         <v/>
       </c>
-      <c r="AD5" s="17" t="str">
-        <f>IF(N5&lt;&gt;"",(N5/$AA5*100)/$Z5,"")</f>
+      <c r="AE5" s="17" t="str">
+        <f>IF(N5&lt;&gt;"",(N5/$AB5*100)/$AA5,"")</f>
         <v/>
       </c>
-      <c r="AE5" s="17" t="e">
-        <f t="shared" ref="AE5" si="1">AVERAGE(AB5:AD5)</f>
+      <c r="AF5" s="17" t="e">
+        <f t="shared" ref="AF5" si="1">AVERAGE(AC5:AE5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AF5" s="17" t="e">
-        <f>STDEV(AB5:AD5)</f>
-        <v>#DIV/0!</v>
-      </c>
       <c r="AG5" s="17" t="e">
-        <f>2^-(J5-T5)</f>
+        <f>STDEV(AC5:AE5)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AH5" s="37" t="str">
@@ -2004,165 +1990,149 @@
         <f t="shared" ref="AL5" si="3">STDEV(AH5:AJ5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AM5" s="17" t="e">
-        <f>O5/AK5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AN5" s="17" t="e">
-        <f t="shared" ref="AN5" si="4">AM5*1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AO5" s="17" t="e">
-        <f>((AL5/AK5)+(P5/O5))*AM5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AP5" s="16" t="e">
-        <f t="shared" ref="AP5" si="5">AO5*1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AQ5" s="35" t="str">
+      <c r="AM5" s="35" t="str">
         <f>C5</f>
         <v>{sampleDate}</v>
       </c>
-      <c r="AR5" s="15" t="s">
+      <c r="AN5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AS5" s="47" t="str">
+      <c r="AO5" s="47" t="str">
         <f>IF(L5&lt;&gt;"",L5/(AK5),"")</f>
         <v/>
       </c>
-      <c r="AT5" s="47" t="str">
+      <c r="AP5" s="47" t="str">
         <f>IF(M5&lt;&gt;"",M5/(AK5),"")</f>
         <v/>
       </c>
-      <c r="AU5" s="47" t="str">
+      <c r="AQ5" s="47" t="str">
         <f>IF(N5&lt;&gt;"",N5/(AK5),"")</f>
         <v/>
       </c>
-      <c r="AV5" s="39" t="e">
-        <f t="shared" ref="AV5" si="6">AVERAGE(AS5:AU5)</f>
+      <c r="AR5" s="39" t="e">
+        <f t="shared" ref="AR5" si="4">AVERAGE(AO5:AQ5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AW5" s="39" t="e">
-        <f t="shared" ref="AW5" si="7">STDEV(AS5:AU5)</f>
+      <c r="AS5" s="39" t="e">
+        <f t="shared" ref="AS5" si="5">STDEV(AO5:AQ5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AX5" s="31" t="str">
-        <f>AB5</f>
-        <v/>
-      </c>
-      <c r="AY5" s="31" t="str">
+      <c r="AT5" s="31" t="str">
         <f>AC5</f>
         <v/>
       </c>
-      <c r="AZ5" s="31" t="str">
+      <c r="AU5" s="31" t="str">
         <f>AD5</f>
         <v/>
       </c>
+      <c r="AV5" s="31" t="str">
+        <f>AE5</f>
+        <v/>
+      </c>
+      <c r="AW5" s="17" t="e">
+        <f t="shared" ref="AW5" si="6">AVERAGE(AT5:AV5)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AX5" s="31" t="str">
+        <f>IF(ISNUMBER(AC5),AC5*$Y5/40*$Z5/$V5*1000,"")</f>
+        <v/>
+      </c>
+      <c r="AY5" s="31" t="str">
+        <f t="shared" ref="AY5:AZ5" si="7">IF(ISNUMBER(AD5),AD5*$Y5/40*$Z5/$V5*1000,"")</f>
+        <v/>
+      </c>
+      <c r="AZ5" s="31" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="BA5" s="17" t="e">
-        <f t="shared" ref="BA5" si="8">AVERAGE(AX5:AZ5)</f>
+        <f>AVERAGE(AX5:AZ5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="BB5" s="31" t="str">
-        <f>IF(ISNUMBER(AB5),AB5*($X5/$Y5*1000),"")</f>
-        <v/>
-      </c>
-      <c r="BC5" s="31" t="str">
-        <f t="shared" ref="BC5:BD5" si="9">IF(ISNUMBER(AC5),AC5*($X5/$Y5*1000),"")</f>
-        <v/>
-      </c>
-      <c r="BD5" s="31" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="BE5" s="17" t="e">
-        <f>AVERAGE(BB5:BD5)</f>
+      <c r="BB5" s="32" t="e">
+        <f>(AK5/1.5*100)/$AA5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="BF5" s="32" t="e">
-        <f>(AK5/1.5*100)/$Z5</f>
+      <c r="BC5" s="33" t="e">
+        <f>BB5*$Y5/40*$Z5/$V5*1000</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="BG5" s="33" t="e">
-        <f>BF5*(X5/Y5*1000)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BH5" s="36" t="str">
-        <f>AQ5</f>
+      <c r="BD5" s="36" t="str">
+        <f>AM5</f>
         <v>{sampleDate}</v>
       </c>
-      <c r="BI5" s="16" t="str">
+      <c r="BE5" s="16" t="str">
         <f>D5</f>
         <v>{sampleID}</v>
       </c>
-      <c r="BJ5" s="16" t="str">
+      <c r="BF5" s="16" t="str">
         <f>IF(Q5&lt;&gt;"",Q5,"")</f>
-        <v>{value_npmmov_dil10_0|}</v>
-      </c>
-      <c r="BK5" s="16" t="str">
+        <v>{value_npmmov_dil10_0|&lt;ND&gt;|&lt;MISSING&gt;}</v>
+      </c>
+      <c r="BG5" s="16" t="str">
         <f>IF(R5&lt;&gt;"",R5,"")</f>
-        <v>{value_npmmov_dil10_1|}</v>
-      </c>
-      <c r="BL5" s="16" t="str">
+        <v>{value_npmmov_dil10_1|&lt;ND&gt;|&lt;MISSING&gt;}</v>
+      </c>
+      <c r="BH5" s="16" t="str">
         <f>IF(S5&lt;&gt;"",S5,"")</f>
-        <v>{value_npmmov_dil10_2|}</v>
-      </c>
-      <c r="BM5" s="16" t="e">
-        <f>AVERAGE(BJ5:BL5)</f>
+        <v>{value_npmmov_dil10_2|&lt;ND&gt;|&lt;MISSING&gt;}</v>
+      </c>
+      <c r="BI5" s="16" t="e">
+        <f>AVERAGE(BF5:BH5)</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="BJ5" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="BK5" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="BL5" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="BM5" s="16" t="str">
+        <f>IF(COUNT(BJ5:BL5)&gt;0,AVERAGE(BJ5:BL5),"")</f>
+        <v/>
+      </c>
       <c r="BN5" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="BO5" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="BP5" s="21" t="s">
-        <v>80</v>
+        <v>98</v>
+      </c>
+      <c r="BO5" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="BP5" s="16" t="s">
+        <v>100</v>
       </c>
       <c r="BQ5" s="16" t="str">
         <f>IF(COUNT(BN5:BP5)&gt;0,AVERAGE(BN5:BP5),"")</f>
         <v/>
       </c>
-      <c r="BR5" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="BS5" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="BT5" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="BU5" s="16" t="str">
-        <f>IF(COUNT(BR5:BT5)&gt;0,AVERAGE(BR5:BT5),"")</f>
+      <c r="BR5" s="16" t="str">
+        <f>IF(AND(ISNUMBER(BI5),ISNUMBER(BQ5)),BI5-BQ5,"")</f>
         <v/>
       </c>
-      <c r="BV5" s="16" t="str">
-        <f>IF(AND(ISNUMBER(BM5),ISNUMBER(BU5)),BM5-BU5,"")</f>
+      <c r="BS5" s="27" t="str">
+        <f>IF(AND(ISNUMBER(BM5),ISNUMBER(BQ5)),BM5-BQ5,"")</f>
         <v/>
       </c>
-      <c r="BW5" s="27" t="str">
-        <f>IF(AND(ISNUMBER(BQ5),ISNUMBER(BU5)),BQ5-BU5,"")</f>
-        <v/>
-      </c>
     </row>
-    <row r="10" spans="1:75" x14ac:dyDescent="0.2">
-      <c r="BS10" s="26"/>
-      <c r="BT10" s="26"/>
-      <c r="BU10" s="26"/>
+    <row r="10" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BO10" s="26"/>
+      <c r="BP10" s="26"/>
+      <c r="BQ10" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="AS3:BD3"/>
-    <mergeCell ref="BH3:BW3"/>
+    <mergeCell ref="AO3:AZ3"/>
+    <mergeCell ref="BD3:BS3"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="AS4:AU4"/>
+    <mergeCell ref="AO4:AQ4"/>
+    <mergeCell ref="AT4:AV4"/>
     <mergeCell ref="AX4:AZ4"/>
-    <mergeCell ref="BB4:BD4"/>
     <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="AC4:AE4"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="I3:K3"/>
   </mergeCells>
@@ -2189,17 +2159,17 @@
       <formula>150</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AS5:AW5">
+  <conditionalFormatting sqref="AO5:AS5">
     <cfRule type="cellIs" dxfId="3" priority="5" operator="lessThan">
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AX5:AZ5 BB5:BD5">
+  <conditionalFormatting sqref="AT5:AV5 AX5:AZ5">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BG5">
+  <conditionalFormatting sqref="BC5">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>100</formula>
     </cfRule>
@@ -2245,7 +2215,7 @@
         <v>31</v>
       </c>
       <c r="G1" s="52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2264,7 +2234,7 @@
       <c r="E2" s="67"/>
       <c r="F2" s="68"/>
       <c r="G2" s="40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2336,7 +2306,7 @@
         <v>29</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G7" s="44" t="e">
         <f ca="1">RSQ(__GETRANGE(cal_row_data, cal_col_ct_avg, __GETCALVAL("Cal-{type}-{plateID}", "num_points")), __GETRANGE(cal_row_data, cal_col_logct, __GETCALVAL("Cal-{type}-{plateID}", "num_points")))*__SETCELL("Cal-{type}-{plateID}", "rsq", 1)</f>

</xml_diff>

<commit_message>
Added __SELECT custom function and updated total volume in Ottawa templates
</commit_message>
<xml_diff>
--- a/qpcr_analyzer/qpcr_template_ottawa.xlsx
+++ b/qpcr_analyzer/qpcr_template_ottawa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinwellman/Documents/Health/Wastewater/Code/odm-qpcr-analyzer/qpcr_analyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B4EFD3-4DA2-CB45-A8CF-2543F50DB6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6362454E-4D72-A442-90A0-AC539CCCA984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{9359BC57-A822-3445-B588-7E071C6D13C9}"/>
   </bookViews>
@@ -343,9 +343,6 @@
     <t>{value_npmmov_2|&lt;ND&gt;|&lt;MISSING&gt;}</t>
   </si>
   <si>
-    <t>{value_totvol_0||}</t>
-  </si>
-  <si>
     <t>{value_emptytubemass_0||}</t>
   </si>
   <si>
@@ -362,6 +359,10 @@
   </si>
   <si>
     <t>main_col_inhibition_40_nodil_dct</t>
+  </si>
+  <si>
+    <t>Sample
+Type</t>
   </si>
 </sst>
 </file>
@@ -771,7 +772,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -925,33 +926,36 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="12" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="12" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -972,6 +976,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1385,10 +1392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A78BE4-03D0-4C45-A8C6-85FB2F5005D2}">
-  <dimension ref="A1:BS10"/>
+  <dimension ref="A1:BT10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AM7" sqref="AM7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1397,39 +1404,36 @@
     <col min="2" max="2" width="8.33203125" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" customWidth="1"/>
     <col min="4" max="4" width="30.1640625" customWidth="1"/>
-    <col min="5" max="6" width="11" customWidth="1"/>
-    <col min="7" max="21" width="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11" customWidth="1"/>
-    <col min="23" max="25" width="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11" customWidth="1"/>
-    <col min="27" max="28" width="16.1640625" customWidth="1"/>
-    <col min="29" max="33" width="11" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="15" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13" customWidth="1"/>
-    <col min="39" max="39" width="13.6640625" customWidth="1"/>
-    <col min="41" max="45" width="11" bestFit="1" customWidth="1"/>
-    <col min="46" max="48" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="13" customWidth="1"/>
-    <col min="50" max="51" width="16.1640625" customWidth="1"/>
-    <col min="52" max="52" width="15.33203125" customWidth="1"/>
-    <col min="53" max="53" width="14.1640625" customWidth="1"/>
-    <col min="54" max="54" width="19.6640625" customWidth="1"/>
-    <col min="55" max="55" width="19.33203125" customWidth="1"/>
-    <col min="56" max="56" width="11" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="29.1640625" customWidth="1"/>
-    <col min="58" max="61" width="11" bestFit="1" customWidth="1"/>
-    <col min="65" max="67" width="11" bestFit="1" customWidth="1"/>
-    <col min="69" max="71" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="11" customWidth="1"/>
+    <col min="8" max="22" width="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" customWidth="1"/>
+    <col min="24" max="26" width="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11" customWidth="1"/>
+    <col min="28" max="29" width="16.1640625" customWidth="1"/>
+    <col min="30" max="34" width="11" bestFit="1" customWidth="1"/>
+    <col min="35" max="37" width="15" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13" customWidth="1"/>
+    <col min="40" max="40" width="13.6640625" customWidth="1"/>
+    <col min="42" max="46" width="11" bestFit="1" customWidth="1"/>
+    <col min="47" max="49" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="13" customWidth="1"/>
+    <col min="51" max="52" width="16.1640625" customWidth="1"/>
+    <col min="53" max="53" width="15.33203125" customWidth="1"/>
+    <col min="54" max="54" width="14.1640625" customWidth="1"/>
+    <col min="55" max="55" width="19.6640625" customWidth="1"/>
+    <col min="56" max="56" width="19.33203125" customWidth="1"/>
+    <col min="57" max="57" width="11" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="29.1640625" customWidth="1"/>
+    <col min="59" max="62" width="11" bestFit="1" customWidth="1"/>
+    <col min="66" max="68" width="11" bestFit="1" customWidth="1"/>
+    <col min="70" max="72" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:72" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>68</v>
       </c>
-      <c r="G1" t="s">
-        <v>49</v>
-      </c>
       <c r="H1" t="s">
         <v>49</v>
       </c>
@@ -1437,22 +1441,22 @@
         <v>49</v>
       </c>
       <c r="J1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" t="s">
         <v>52</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="N1" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>50</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>53</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>51</v>
       </c>
       <c r="R1" t="s">
         <v>51</v>
@@ -1461,10 +1465,10 @@
         <v>51</v>
       </c>
       <c r="T1" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" t="s">
         <v>66</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>55</v>
       </c>
       <c r="AD1" t="s">
         <v>55</v>
@@ -1473,10 +1477,10 @@
         <v>55</v>
       </c>
       <c r="AF1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG1" t="s">
         <v>54</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>57</v>
       </c>
       <c r="AP1" t="s">
         <v>57</v>
@@ -1485,10 +1489,10 @@
         <v>57</v>
       </c>
       <c r="AR1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AS1" t="s">
         <v>56</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>58</v>
       </c>
       <c r="AY1" t="s">
         <v>58</v>
@@ -1497,10 +1501,10 @@
         <v>58</v>
       </c>
       <c r="BA1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BB1" t="s">
         <v>59</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>60</v>
       </c>
       <c r="BG1" t="s">
         <v>60</v>
@@ -1509,10 +1513,10 @@
         <v>60</v>
       </c>
       <c r="BI1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" t="s">
         <v>61</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>63</v>
       </c>
       <c r="BK1" t="s">
         <v>63</v>
@@ -1521,10 +1525,10 @@
         <v>63</v>
       </c>
       <c r="BM1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BN1" t="s">
         <v>62</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>65</v>
       </c>
       <c r="BO1" t="s">
         <v>65</v>
@@ -1533,16 +1537,19 @@
         <v>65</v>
       </c>
       <c r="BQ1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BR1" t="s">
         <v>64</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
+        <v>105</v>
+      </c>
+      <c r="BT1" t="s">
         <v>106</v>
       </c>
-      <c r="BS1" t="s">
-        <v>107</v>
-      </c>
     </row>
-    <row r="2" spans="1:71" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:72" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
@@ -1600,8 +1607,8 @@
       <c r="BA2" s="1"/>
       <c r="BB2" s="1"/>
       <c r="BC2" s="1"/>
-      <c r="BD2" s="2"/>
-      <c r="BE2" s="3"/>
+      <c r="BD2" s="1"/>
+      <c r="BE2" s="2"/>
       <c r="BF2" s="3"/>
       <c r="BG2" s="3"/>
       <c r="BH2" s="3"/>
@@ -1615,9 +1622,10 @@
       <c r="BP2" s="3"/>
       <c r="BQ2" s="3"/>
       <c r="BR2" s="3"/>
-      <c r="BS2" s="4"/>
+      <c r="BS2" s="3"/>
+      <c r="BT2" s="4"/>
     </row>
-    <row r="3" spans="1:71" s="5" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:72" s="5" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
@@ -1628,56 +1636,57 @@
         <v>0</v>
       </c>
       <c r="D3" s="41"/>
-      <c r="E3" s="64" t="e">
+      <c r="E3" s="65" t="e">
         <f ca="1">__QAQCHASFAILEDCATEGORY("NTC", "NTC Error! See {qaqc_sheet}", "NTCs Good", "No NTCs")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="65" t="e">
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="66" t="e">
         <f ca="1">__QAQCHASFAILEDCATEGORY("EB", "EB Error! See {qaqc_sheet}", "Extraction Blanks Good", "No Extraction Blanks")</f>
         <v>#NAME?</v>
       </c>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="AO3" s="53" t="s">
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="51"/>
+      <c r="AP3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="AP3" s="54"/>
-      <c r="AQ3" s="54"/>
-      <c r="AR3" s="54"/>
-      <c r="AS3" s="54"/>
-      <c r="AT3" s="54"/>
-      <c r="AU3" s="54"/>
-      <c r="AV3" s="54"/>
-      <c r="AW3" s="54"/>
-      <c r="AX3" s="54"/>
-      <c r="AY3" s="54"/>
+      <c r="AQ3" s="55"/>
+      <c r="AR3" s="55"/>
+      <c r="AS3" s="55"/>
+      <c r="AT3" s="55"/>
+      <c r="AU3" s="55"/>
+      <c r="AV3" s="55"/>
+      <c r="AW3" s="55"/>
+      <c r="AX3" s="55"/>
+      <c r="AY3" s="55"/>
       <c r="AZ3" s="55"/>
-      <c r="BA3" s="28"/>
-      <c r="BB3" s="29"/>
-      <c r="BC3" s="30"/>
-      <c r="BD3" s="56" t="s">
+      <c r="BA3" s="56"/>
+      <c r="BB3" s="28"/>
+      <c r="BC3" s="29"/>
+      <c r="BD3" s="30"/>
+      <c r="BE3" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="BE3" s="56"/>
-      <c r="BF3" s="56"/>
-      <c r="BG3" s="56"/>
-      <c r="BH3" s="56"/>
-      <c r="BI3" s="56"/>
-      <c r="BJ3" s="56"/>
-      <c r="BK3" s="56"/>
-      <c r="BL3" s="56"/>
-      <c r="BM3" s="56"/>
-      <c r="BN3" s="56"/>
-      <c r="BO3" s="56"/>
-      <c r="BP3" s="56"/>
-      <c r="BQ3" s="56"/>
-      <c r="BR3" s="56"/>
+      <c r="BF3" s="57"/>
+      <c r="BG3" s="57"/>
+      <c r="BH3" s="57"/>
+      <c r="BI3" s="57"/>
+      <c r="BJ3" s="57"/>
+      <c r="BK3" s="57"/>
+      <c r="BL3" s="57"/>
+      <c r="BM3" s="57"/>
+      <c r="BN3" s="57"/>
+      <c r="BO3" s="57"/>
+      <c r="BP3" s="57"/>
+      <c r="BQ3" s="57"/>
+      <c r="BR3" s="57"/>
       <c r="BS3" s="57"/>
+      <c r="BT3" s="58"/>
     </row>
-    <row r="4" spans="1:71" s="5" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:72" s="5" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1693,129 +1702,129 @@
       <c r="F4" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="G4" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="59"/>
       <c r="I4" s="60"/>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="61"/>
+      <c r="K4" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="L4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="58" t="s">
+      <c r="M4" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="59"/>
       <c r="N4" s="60"/>
-      <c r="O4" s="8" t="s">
+      <c r="O4" s="61"/>
+      <c r="P4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="Q4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="Q4" s="58" t="s">
+      <c r="R4" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="R4" s="59"/>
       <c r="S4" s="60"/>
-      <c r="T4" s="8" t="s">
+      <c r="T4" s="61"/>
+      <c r="U4" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="U4" s="7" t="s">
+      <c r="V4" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="V4" s="7" t="s">
+      <c r="W4" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="W4" s="7" t="s">
+      <c r="X4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="X4" s="7" t="s">
+      <c r="Y4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Y4" s="7" t="s">
+      <c r="Z4" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="Z4" s="7" t="s">
+      <c r="AA4" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="AA4" s="7" t="s">
+      <c r="AB4" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="AB4" s="48" t="s">
+      <c r="AC4" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="AC4" s="61" t="s">
+      <c r="AD4" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="AD4" s="62"/>
       <c r="AE4" s="63"/>
-      <c r="AF4" s="9" t="s">
+      <c r="AF4" s="64"/>
+      <c r="AG4" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="AG4" s="7" t="s">
+      <c r="AH4" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AH4" s="61" t="s">
+      <c r="AI4" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="AI4" s="62"/>
       <c r="AJ4" s="63"/>
-      <c r="AK4" s="7" t="s">
+      <c r="AK4" s="64"/>
+      <c r="AL4" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="AL4" s="7" t="s">
+      <c r="AM4" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AM4" s="6" t="s">
+      <c r="AN4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="AN4" s="6" t="s">
+      <c r="AO4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AO4" s="61" t="s">
+      <c r="AP4" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="AP4" s="62"/>
       <c r="AQ4" s="63"/>
-      <c r="AR4" s="18" t="s">
+      <c r="AR4" s="64"/>
+      <c r="AS4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="AS4" s="18" t="s">
+      <c r="AT4" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="AT4" s="61" t="s">
+      <c r="AU4" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="AU4" s="62"/>
       <c r="AV4" s="63"/>
-      <c r="AW4" s="7" t="s">
+      <c r="AW4" s="64"/>
+      <c r="AX4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="AX4" s="61" t="s">
+      <c r="AY4" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="AY4" s="62"/>
       <c r="AZ4" s="63"/>
-      <c r="BA4" s="19" t="s">
+      <c r="BA4" s="64"/>
+      <c r="BB4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="BB4" s="10" t="s">
+      <c r="BC4" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="BC4" s="11" t="s">
+      <c r="BD4" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="BD4" s="20" t="s">
+      <c r="BE4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="BE4" s="12" t="s">
+      <c r="BF4" s="12" t="s">
         <v>12</v>
-      </c>
-      <c r="BF4" s="12" t="s">
-        <v>83</v>
       </c>
       <c r="BG4" s="12" t="s">
         <v>83</v>
@@ -1823,11 +1832,11 @@
       <c r="BH4" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="BI4" s="13" t="s">
+      <c r="BI4" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="BJ4" s="13" t="s">
         <v>13</v>
-      </c>
-      <c r="BJ4" s="12" t="s">
-        <v>84</v>
       </c>
       <c r="BK4" s="12" t="s">
         <v>84</v>
@@ -1835,11 +1844,11 @@
       <c r="BL4" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="BM4" s="13" t="s">
+      <c r="BM4" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="BN4" s="13" t="s">
         <v>14</v>
-      </c>
-      <c r="BN4" s="12" t="s">
-        <v>85</v>
       </c>
       <c r="BO4" s="12" t="s">
         <v>85</v>
@@ -1847,17 +1856,20 @@
       <c r="BP4" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="BQ4" s="13" t="s">
+      <c r="BQ4" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="BR4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="BR4" s="12" t="s">
+      <c r="BS4" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="BS4" s="14" t="s">
+      <c r="BT4" s="14" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:71" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:72" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1873,26 +1885,26 @@
       <c r="F5" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="15" t="e">
+        <f ca="1">__QUOTIFY(__GETDATA(D5, "sample_typeShortDescription"))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H5" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="I5" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="J5" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="J5" s="16" t="e">
-        <f>AVERAGE(G5:I5)</f>
+      <c r="K5" s="16" t="e">
+        <f>AVERAGE(H5:J5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K5" s="16" t="e">
-        <f>STDEV(G5:I5)</f>
+      <c r="L5" s="16" t="e">
+        <f>STDEV(H5:J5)</f>
         <v>#DIV/0!</v>
-      </c>
-      <c r="L5" s="38" t="str">
-        <f>IF(ISNUMBER(G5),10^((G5-__GETCELL(__GETDATA(G5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(G5, "standardCurveID"), "slope", FALSE)),"")</f>
-        <v/>
       </c>
       <c r="M5" s="38" t="str">
         <f>IF(ISNUMBER(H5),10^((H5-__GETCELL(__GETDATA(H5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(H5, "standardCurveID"), "slope", FALSE)),"")</f>
@@ -1902,77 +1914,78 @@
         <f>IF(ISNUMBER(I5),10^((I5-__GETCELL(__GETDATA(I5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(I5, "standardCurveID"), "slope", FALSE)),"")</f>
         <v/>
       </c>
-      <c r="O5" s="16" t="e">
-        <f>AVERAGE(L5:N5)</f>
+      <c r="O5" s="38" t="str">
+        <f>IF(ISNUMBER(J5),10^((J5-__GETCELL(__GETDATA(J5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(J5, "standardCurveID"), "slope", FALSE)),"")</f>
+        <v/>
+      </c>
+      <c r="P5" s="16" t="e">
+        <f>AVERAGE(M5:O5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="P5" s="16" t="e">
-        <f>STDEV(L5:N5)</f>
+      <c r="Q5" s="16" t="e">
+        <f>STDEV(M5:O5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q5" s="16" t="s">
+      <c r="R5" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="R5" s="16" t="s">
+      <c r="S5" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="S5" s="16" t="s">
+      <c r="T5" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="T5" s="16" t="e">
-        <f>AVERAGE(Q5:S5)</f>
+      <c r="U5" s="16" t="e">
+        <f>AVERAGE(R5:T5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U5" s="16" t="e">
-        <f t="shared" ref="U5" si="0">STDEV(Q5:S5)</f>
+      <c r="V5" s="16" t="e">
+        <f t="shared" ref="V5" si="0">STDEV(R5:T5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="V5" s="17" t="s">
+      <c r="W5" s="17" t="e">
+        <f ca="1">IF(G5="PS",40,__SELECT("{value_totvol_0||}", """"))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="X5" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="W5" s="17" t="s">
+      <c r="Y5" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="X5" s="17" t="s">
+      <c r="Z5" s="17" t="e">
+        <f>IF(AND(Y5&lt;&gt;"",X5&lt;&gt;""),Y5-X5,"")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AA5" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="Y5" s="17" t="e">
-        <f>IF(AND(X5&lt;&gt;"",W5&lt;&gt;""),X5-W5,"")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Z5" s="17" t="s">
+      <c r="AB5" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="AA5" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB5" s="49">
+      <c r="AC5" s="49">
         <f>IF(ISERROR(DATEVALUE(B5)),3,IF(DATEVALUE(B5)&gt;=DATE(2021,6,8),3,1.5))</f>
         <v>3</v>
       </c>
-      <c r="AC5" s="17" t="str">
-        <f>IF(L5&lt;&gt;"",(L5/$AB5*100)/$AA5,"")</f>
+      <c r="AD5" s="17" t="str">
+        <f>IF(M5&lt;&gt;"",(M5/$AC5*100)/$AB5,"")</f>
         <v/>
       </c>
-      <c r="AD5" s="17" t="str">
-        <f>IF(M5&lt;&gt;"",(M5/$AB5*100)/$AA5,"")</f>
+      <c r="AE5" s="17" t="str">
+        <f>IF(N5&lt;&gt;"",(N5/$AC5*100)/$AB5,"")</f>
         <v/>
       </c>
-      <c r="AE5" s="17" t="str">
-        <f>IF(N5&lt;&gt;"",(N5/$AB5*100)/$AA5,"")</f>
+      <c r="AF5" s="17" t="str">
+        <f>IF(O5&lt;&gt;"",(O5/$AC5*100)/$AB5,"")</f>
         <v/>
       </c>
-      <c r="AF5" s="17" t="e">
-        <f t="shared" ref="AF5" si="1">AVERAGE(AC5:AE5)</f>
+      <c r="AG5" s="17" t="e">
+        <f t="shared" ref="AG5" si="1">AVERAGE(AD5:AF5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AG5" s="17" t="e">
-        <f>STDEV(AC5:AE5)</f>
+      <c r="AH5" s="17" t="e">
+        <f>STDEV(AD5:AF5)</f>
         <v>#DIV/0!</v>
-      </c>
-      <c r="AH5" s="37" t="str">
-        <f>IF(ISNUMBER(Q5),10^((Q5-__GETCELL(__GETDATA(Q5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(Q5,"standardCurveID"), "slope", FALSE)),"")</f>
-        <v/>
       </c>
       <c r="AI5" s="37" t="str">
         <f>IF(ISNUMBER(R5),10^((R5-__GETCELL(__GETDATA(R5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(R5,"standardCurveID"), "slope", FALSE)),"")</f>
@@ -1982,44 +1995,44 @@
         <f>IF(ISNUMBER(S5),10^((S5-__GETCELL(__GETDATA(S5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(S5,"standardCurveID"), "slope", FALSE)),"")</f>
         <v/>
       </c>
-      <c r="AK5" s="46" t="e">
-        <f t="shared" ref="AK5" si="2">AVERAGE(AH5:AJ5)*10</f>
+      <c r="AK5" s="37" t="str">
+        <f>IF(ISNUMBER(T5),10^((T5-__GETCELL(__GETDATA(T5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(T5,"standardCurveID"), "slope", FALSE)),"")</f>
+        <v/>
+      </c>
+      <c r="AL5" s="46" t="e">
+        <f t="shared" ref="AL5" si="2">AVERAGE(AI5:AK5)*10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AL5" s="17" t="e">
-        <f t="shared" ref="AL5" si="3">STDEV(AH5:AJ5)</f>
+      <c r="AM5" s="17" t="e">
+        <f t="shared" ref="AM5" si="3">STDEV(AI5:AK5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AM5" s="35" t="str">
+      <c r="AN5" s="35" t="str">
         <f>C5</f>
         <v>{sampleDate}</v>
       </c>
-      <c r="AN5" s="15" t="s">
+      <c r="AO5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AO5" s="47" t="str">
-        <f>IF(L5&lt;&gt;"",L5/(AK5),"")</f>
+      <c r="AP5" s="47" t="str">
+        <f>IF(M5&lt;&gt;"",M5/(AL5),"")</f>
         <v/>
       </c>
-      <c r="AP5" s="47" t="str">
-        <f>IF(M5&lt;&gt;"",M5/(AK5),"")</f>
+      <c r="AQ5" s="47" t="str">
+        <f>IF(N5&lt;&gt;"",N5/(AL5),"")</f>
         <v/>
       </c>
-      <c r="AQ5" s="47" t="str">
-        <f>IF(N5&lt;&gt;"",N5/(AK5),"")</f>
+      <c r="AR5" s="47" t="str">
+        <f>IF(O5&lt;&gt;"",O5/(AL5),"")</f>
         <v/>
       </c>
-      <c r="AR5" s="39" t="e">
-        <f t="shared" ref="AR5" si="4">AVERAGE(AO5:AQ5)</f>
+      <c r="AS5" s="39" t="e">
+        <f t="shared" ref="AS5" si="4">AVERAGE(AP5:AR5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AS5" s="39" t="e">
-        <f t="shared" ref="AS5" si="5">STDEV(AO5:AQ5)</f>
+      <c r="AT5" s="39" t="e">
+        <f t="shared" ref="AT5" si="5">STDEV(AP5:AR5)</f>
         <v>#DIV/0!</v>
-      </c>
-      <c r="AT5" s="31" t="str">
-        <f>AC5</f>
-        <v/>
       </c>
       <c r="AU5" s="31" t="str">
         <f>AD5</f>
@@ -2029,114 +2042,118 @@
         <f>AE5</f>
         <v/>
       </c>
-      <c r="AW5" s="17" t="e">
-        <f t="shared" ref="AW5" si="6">AVERAGE(AT5:AV5)</f>
+      <c r="AW5" s="31" t="str">
+        <f>AF5</f>
+        <v/>
+      </c>
+      <c r="AX5" s="17" t="e">
+        <f t="shared" ref="AX5" si="6">AVERAGE(AU5:AW5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AX5" s="31" t="str">
-        <f>IF(ISNUMBER(AC5),AC5*$Y5/40*$Z5/$V5*1000,"")</f>
+      <c r="AY5" s="31" t="str">
+        <f>IF(ISNUMBER(AD5),AD5*$Z5/40*$AA5/$W5*1000,"")</f>
         <v/>
       </c>
-      <c r="AY5" s="31" t="str">
-        <f t="shared" ref="AY5:AZ5" si="7">IF(ISNUMBER(AD5),AD5*$Y5/40*$Z5/$V5*1000,"")</f>
+      <c r="AZ5" s="31" t="str">
+        <f t="shared" ref="AZ5:BA5" si="7">IF(ISNUMBER(AE5),AE5*$Z5/40*$AA5/$W5*1000,"")</f>
         <v/>
       </c>
-      <c r="AZ5" s="31" t="str">
+      <c r="BA5" s="31" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="BA5" s="17" t="e">
-        <f>AVERAGE(AX5:AZ5)</f>
+      <c r="BB5" s="17" t="e">
+        <f>AVERAGE(AY5:BA5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="BB5" s="32" t="e">
-        <f>(AK5/1.5*100)/$AA5</f>
+      <c r="BC5" s="32" t="e">
+        <f>(AL5/1.5*100)/$AB5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="BC5" s="33" t="e">
-        <f>BB5*$Y5/40*$Z5/$V5*1000</f>
+      <c r="BD5" s="33" t="e">
+        <f ca="1">BC5*$Z5/40*$AA5/$W5*1000</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="BD5" s="36" t="str">
-        <f>AM5</f>
+      <c r="BE5" s="36" t="str">
+        <f>AN5</f>
         <v>{sampleDate}</v>
       </c>
-      <c r="BE5" s="16" t="str">
+      <c r="BF5" s="16" t="str">
         <f>D5</f>
         <v>{sampleID}</v>
       </c>
-      <c r="BF5" s="16" t="str">
-        <f>IF(Q5&lt;&gt;"",Q5,"")</f>
-        <v>{value_npmmov_dil10_0|&lt;ND&gt;|&lt;MISSING&gt;}</v>
-      </c>
       <c r="BG5" s="16" t="str">
         <f>IF(R5&lt;&gt;"",R5,"")</f>
-        <v>{value_npmmov_dil10_1|&lt;ND&gt;|&lt;MISSING&gt;}</v>
+        <v>{value_npmmov_dil10_0|&lt;ND&gt;|&lt;MISSING&gt;}</v>
       </c>
       <c r="BH5" s="16" t="str">
         <f>IF(S5&lt;&gt;"",S5,"")</f>
+        <v>{value_npmmov_dil10_1|&lt;ND&gt;|&lt;MISSING&gt;}</v>
+      </c>
+      <c r="BI5" s="16" t="str">
+        <f>IF(T5&lt;&gt;"",T5,"")</f>
         <v>{value_npmmov_dil10_2|&lt;ND&gt;|&lt;MISSING&gt;}</v>
       </c>
-      <c r="BI5" s="16" t="e">
-        <f>AVERAGE(BF5:BH5)</f>
+      <c r="BJ5" s="16" t="e">
+        <f>AVERAGE(BG5:BI5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="BJ5" s="16" t="s">
+      <c r="BK5" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="BK5" s="21" t="s">
+      <c r="BL5" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="BL5" s="21" t="s">
+      <c r="BM5" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="BM5" s="16" t="str">
-        <f>IF(COUNT(BJ5:BL5)&gt;0,AVERAGE(BJ5:BL5),"")</f>
+      <c r="BN5" s="16" t="str">
+        <f>IF(COUNT(BK5:BM5)&gt;0,AVERAGE(BK5:BM5),"")</f>
         <v/>
       </c>
-      <c r="BN5" s="16" t="s">
+      <c r="BO5" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="BO5" s="16" t="s">
+      <c r="BP5" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="BP5" s="16" t="s">
+      <c r="BQ5" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="BQ5" s="16" t="str">
-        <f>IF(COUNT(BN5:BP5)&gt;0,AVERAGE(BN5:BP5),"")</f>
+      <c r="BR5" s="16" t="str">
+        <f>IF(COUNT(BO5:BQ5)&gt;0,AVERAGE(BO5:BQ5),"")</f>
         <v/>
       </c>
-      <c r="BR5" s="16" t="str">
-        <f>IF(AND(ISNUMBER(BI5),ISNUMBER(BQ5)),BI5-BQ5,"")</f>
+      <c r="BS5" s="16" t="str">
+        <f>IF(AND(ISNUMBER(BJ5),ISNUMBER(BR5)),BJ5-BR5,"")</f>
         <v/>
       </c>
-      <c r="BS5" s="27" t="str">
-        <f>IF(AND(ISNUMBER(BM5),ISNUMBER(BQ5)),BM5-BQ5,"")</f>
+      <c r="BT5" s="27" t="str">
+        <f>IF(AND(ISNUMBER(BN5),ISNUMBER(BR5)),BN5-BR5,"")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:71" x14ac:dyDescent="0.2">
-      <c r="BO10" s="26"/>
+    <row r="10" spans="1:72" x14ac:dyDescent="0.2">
       <c r="BP10" s="26"/>
       <c r="BQ10" s="26"/>
+      <c r="BR10" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="AO3:AZ3"/>
-    <mergeCell ref="BD3:BS3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="AO4:AQ4"/>
-    <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AX4:AZ4"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AC4:AE4"/>
+    <mergeCell ref="AP3:BA3"/>
+    <mergeCell ref="BE3:BT3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AU4:AW4"/>
+    <mergeCell ref="AY4:BA4"/>
+    <mergeCell ref="AI4:AK4"/>
+    <mergeCell ref="AD4:AF4"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="I3:K3"/>
   </mergeCells>
-  <conditionalFormatting sqref="L5:N5">
+  <conditionalFormatting sqref="M5:O5">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="lessThan">
       <formula>3.75</formula>
     </cfRule>
@@ -2145,13 +2162,13 @@
       <formula>$C$1564</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH5:AJ5">
+  <conditionalFormatting sqref="AI5:AK5">
     <cfRule type="cellIs" dxfId="6" priority="8" operator="between">
-      <formula>$AH$2697</formula>
-      <formula>$AH$2701</formula>
+      <formula>$AI$2697</formula>
+      <formula>$AI$2701</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH5:AJ5">
+  <conditionalFormatting sqref="AI5:AK5">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
       <formula>38894</formula>
     </cfRule>
@@ -2159,22 +2176,22 @@
       <formula>150</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AO5:AS5">
+  <conditionalFormatting sqref="AP5:AT5">
     <cfRule type="cellIs" dxfId="3" priority="5" operator="lessThan">
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AT5:AV5 AX5:AZ5">
+  <conditionalFormatting sqref="AU5:AW5 AY5:BA5">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BC5">
+  <conditionalFormatting sqref="BD5">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L5:N5">
+  <conditionalFormatting sqref="M5:O5">
     <cfRule type="cellIs" dxfId="0" priority="12" operator="between">
       <formula>#REF!</formula>
       <formula>#REF!</formula>
@@ -2228,11 +2245,11 @@
       <c r="C2" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="67"/>
-      <c r="F2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="69"/>
       <c r="G2" s="40" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
QPCRUpdater deletes trailing blank rows, updated calibration templates to show ND and MISSING
</commit_message>
<xml_diff>
--- a/qpcr_analyzer/qpcr_template_ottawa.xlsx
+++ b/qpcr_analyzer/qpcr_template_ottawa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinwellman/Documents/Health/Wastewater/Code/odm-qpcr-analyzer/qpcr_analyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6362454E-4D72-A442-90A0-AC539CCCA984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF0A003-3406-7A4D-A38A-C65A4162C7D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{9359BC57-A822-3445-B588-7E071C6D13C9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="1" xr2:uid="{9359BC57-A822-3445-B588-7E071C6D13C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="105">
   <si>
     <t>qPCR Data</t>
   </si>
@@ -122,15 +122,6 @@
   </si>
   <si>
     <t>cal_col_ct</t>
-  </si>
-  <si>
-    <t>{value_0}</t>
-  </si>
-  <si>
-    <t>{value_1}</t>
-  </si>
-  <si>
-    <t>{value_2}</t>
   </si>
   <si>
     <t>{value_sq_avg}</t>
@@ -929,6 +920,9 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="12" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -976,9 +970,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1394,7 +1385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A78BE4-03D0-4C45-A8C6-85FB2F5005D2}">
   <dimension ref="A1:BT10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E3" sqref="E3:G3"/>
     </sheetView>
   </sheetViews>
@@ -1432,121 +1423,121 @@
   <sheetData>
     <row r="1" spans="1:72" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S1" t="s">
+        <v>48</v>
+      </c>
+      <c r="T1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD1" t="s">
         <v>52</v>
       </c>
-      <c r="M1" t="s">
-        <v>50</v>
-      </c>
-      <c r="N1" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="O1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="AE1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS1" t="s">
         <v>53</v>
       </c>
-      <c r="R1" t="s">
-        <v>51</v>
-      </c>
-      <c r="S1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T1" t="s">
-        <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD1" t="s">
+      <c r="AY1" t="s">
         <v>55</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AZ1" t="s">
         <v>55</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="BA1" t="s">
         <v>55</v>
       </c>
-      <c r="AG1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AP1" t="s">
+      <c r="BB1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BG1" t="s">
         <v>57</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="BH1" t="s">
         <v>57</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="BI1" t="s">
         <v>57</v>
       </c>
-      <c r="AS1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AY1" t="s">
+      <c r="BJ1" t="s">
         <v>58</v>
       </c>
-      <c r="AZ1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BB1" t="s">
+      <c r="BK1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BN1" t="s">
         <v>59</v>
       </c>
-      <c r="BG1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BJ1" t="s">
+      <c r="BO1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BR1" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>64</v>
-      </c>
       <c r="BS1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="BT1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:72" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1630,61 +1621,61 @@
         <v>24</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="41"/>
-      <c r="E3" s="65" t="e">
+      <c r="E3" s="66" t="e">
         <f ca="1">__QAQCHASFAILEDCATEGORY("NTC", "NTC Error! See {qaqc_sheet}", "NTCs Good", "No NTCs")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="66" t="e">
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="67" t="e">
         <f ca="1">__QAQCHASFAILEDCATEGORY("EB", "EB Error! See {qaqc_sheet}", "Extraction Blanks Good", "No Extraction Blanks")</f>
         <v>#NAME?</v>
       </c>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
       <c r="L3" s="51"/>
-      <c r="AP3" s="54" t="s">
+      <c r="AP3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="AQ3" s="55"/>
-      <c r="AR3" s="55"/>
-      <c r="AS3" s="55"/>
-      <c r="AT3" s="55"/>
-      <c r="AU3" s="55"/>
-      <c r="AV3" s="55"/>
-      <c r="AW3" s="55"/>
-      <c r="AX3" s="55"/>
-      <c r="AY3" s="55"/>
-      <c r="AZ3" s="55"/>
-      <c r="BA3" s="56"/>
+      <c r="AQ3" s="56"/>
+      <c r="AR3" s="56"/>
+      <c r="AS3" s="56"/>
+      <c r="AT3" s="56"/>
+      <c r="AU3" s="56"/>
+      <c r="AV3" s="56"/>
+      <c r="AW3" s="56"/>
+      <c r="AX3" s="56"/>
+      <c r="AY3" s="56"/>
+      <c r="AZ3" s="56"/>
+      <c r="BA3" s="57"/>
       <c r="BB3" s="28"/>
       <c r="BC3" s="29"/>
       <c r="BD3" s="30"/>
-      <c r="BE3" s="57" t="s">
+      <c r="BE3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="BF3" s="57"/>
-      <c r="BG3" s="57"/>
-      <c r="BH3" s="57"/>
-      <c r="BI3" s="57"/>
-      <c r="BJ3" s="57"/>
-      <c r="BK3" s="57"/>
-      <c r="BL3" s="57"/>
-      <c r="BM3" s="57"/>
-      <c r="BN3" s="57"/>
-      <c r="BO3" s="57"/>
-      <c r="BP3" s="57"/>
-      <c r="BQ3" s="57"/>
-      <c r="BR3" s="57"/>
-      <c r="BS3" s="57"/>
-      <c r="BT3" s="58"/>
+      <c r="BF3" s="58"/>
+      <c r="BG3" s="58"/>
+      <c r="BH3" s="58"/>
+      <c r="BI3" s="58"/>
+      <c r="BJ3" s="58"/>
+      <c r="BK3" s="58"/>
+      <c r="BL3" s="58"/>
+      <c r="BM3" s="58"/>
+      <c r="BN3" s="58"/>
+      <c r="BO3" s="58"/>
+      <c r="BP3" s="58"/>
+      <c r="BQ3" s="58"/>
+      <c r="BR3" s="58"/>
+      <c r="BS3" s="58"/>
+      <c r="BT3" s="59"/>
     </row>
     <row r="4" spans="1:72" s="5" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
@@ -1697,49 +1688,49 @@
         <v>4</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F4" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="53" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="61"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="61"/>
+      <c r="O4" s="62"/>
+      <c r="P4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R4" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="S4" s="61"/>
+      <c r="T4" s="62"/>
+      <c r="U4" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="53" t="s">
-        <v>107</v>
-      </c>
-      <c r="H4" s="59" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="M4" s="59" t="s">
-        <v>6</v>
-      </c>
-      <c r="N4" s="60"/>
-      <c r="O4" s="61"/>
-      <c r="P4" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="R4" s="59" t="s">
-        <v>74</v>
-      </c>
-      <c r="S4" s="60"/>
-      <c r="T4" s="61"/>
-      <c r="U4" s="8" t="s">
-        <v>75</v>
-      </c>
       <c r="V4" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="W4" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X4" s="7" t="s">
         <v>7</v>
@@ -1748,77 +1739,77 @@
         <v>8</v>
       </c>
       <c r="Z4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA4" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC4" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD4" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE4" s="64"/>
+      <c r="AF4" s="65"/>
+      <c r="AG4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH4" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AA4" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB4" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC4" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="AD4" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE4" s="63"/>
-      <c r="AF4" s="64"/>
-      <c r="AG4" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH4" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI4" s="62" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ4" s="63"/>
-      <c r="AK4" s="64"/>
+      <c r="AI4" s="63" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ4" s="64"/>
+      <c r="AK4" s="65"/>
       <c r="AL4" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="AM4" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AN4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="AO4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP4" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="AQ4" s="63"/>
-      <c r="AR4" s="64"/>
+        <v>37</v>
+      </c>
+      <c r="AP4" s="63" t="s">
+        <v>77</v>
+      </c>
+      <c r="AQ4" s="64"/>
+      <c r="AR4" s="65"/>
       <c r="AS4" s="18" t="s">
         <v>10</v>
       </c>
       <c r="AT4" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="AU4" s="62" t="s">
-        <v>46</v>
-      </c>
-      <c r="AV4" s="63"/>
-      <c r="AW4" s="64"/>
+        <v>42</v>
+      </c>
+      <c r="AU4" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="AV4" s="64"/>
+      <c r="AW4" s="65"/>
       <c r="AX4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="AY4" s="62" t="s">
+      <c r="AY4" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="AZ4" s="63"/>
-      <c r="BA4" s="64"/>
+      <c r="AZ4" s="64"/>
+      <c r="BA4" s="65"/>
       <c r="BB4" s="19" t="s">
         <v>10</v>
       </c>
       <c r="BC4" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="BD4" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="BE4" s="20" t="s">
         <v>3</v>
@@ -1827,46 +1818,46 @@
         <v>12</v>
       </c>
       <c r="BG4" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="BH4" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="BI4" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="BJ4" s="13" t="s">
         <v>13</v>
       </c>
       <c r="BK4" s="12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="BL4" s="12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="BM4" s="12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="BN4" s="13" t="s">
         <v>14</v>
       </c>
       <c r="BO4" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="BP4" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="BQ4" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="BR4" s="13" t="s">
         <v>15</v>
       </c>
       <c r="BS4" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="BT4" s="14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:72" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1883,20 +1874,20 @@
         <v>23</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G5" s="15" t="e">
         <f ca="1">__QUOTIFY(__GETDATA(D5, "sample_typeShortDescription"))</f>
         <v>#NAME?</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K5" s="16" t="e">
         <f>AVERAGE(H5:J5)</f>
@@ -1927,13 +1918,13 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R5" s="16" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="S5" s="16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="T5" s="16" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="U5" s="16" t="e">
         <f>AVERAGE(R5:T5)</f>
@@ -1948,20 +1939,20 @@
         <v>#NAME?</v>
       </c>
       <c r="X5" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="Y5" s="17" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Z5" s="17" t="e">
         <f>IF(AND(Y5&lt;&gt;"",X5&lt;&gt;""),Y5-X5,"")</f>
         <v>#VALUE!</v>
       </c>
       <c r="AA5" s="17" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="AB5" s="17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="AC5" s="49">
         <f>IF(ISERROR(DATEVALUE(B5)),3,IF(DATEVALUE(B5)&gt;=DATE(2021,6,8),3,1.5))</f>
@@ -2099,26 +2090,26 @@
         <v>#DIV/0!</v>
       </c>
       <c r="BK5" s="16" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="BL5" s="21" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="BM5" s="21" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="BN5" s="16" t="str">
         <f>IF(COUNT(BK5:BM5)&gt;0,AVERAGE(BK5:BM5),"")</f>
         <v/>
       </c>
       <c r="BO5" s="16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="BP5" s="16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="BQ5" s="16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="BR5" s="16" t="str">
         <f>IF(COUNT(BO5:BQ5)&gt;0,AVERAGE(BO5:BQ5),"")</f>
@@ -2140,6 +2131,8 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
     <mergeCell ref="AP3:BA3"/>
     <mergeCell ref="BE3:BT3"/>
     <mergeCell ref="H4:J4"/>
@@ -2150,8 +2143,6 @@
     <mergeCell ref="AY4:BA4"/>
     <mergeCell ref="AI4:AK4"/>
     <mergeCell ref="AD4:AF4"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
   </mergeCells>
   <conditionalFormatting sqref="M5:O5">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="lessThan">
@@ -2206,8 +2197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43405FCF-EE9C-0146-81B2-A2A958472A61}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScale="103" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2232,7 +2223,7 @@
         <v>31</v>
       </c>
       <c r="G1" s="52" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2245,13 +2236,13 @@
       <c r="C2" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="68"/>
-      <c r="F2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="70"/>
       <c r="G2" s="40" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2259,20 +2250,20 @@
         <v>28</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C3" s="24" t="e">
         <f>LOG(B3)</f>
         <v>#VALUE!</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="G3" s="22" t="e">
         <f ca="1">AVERAGE(D3:F3)*__SETCELL("Cal-{type}-{plateID}", "avg_std_#",1)</f>
@@ -2323,7 +2314,7 @@
         <v>29</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G7" s="44" t="e">
         <f ca="1">RSQ(__GETRANGE(cal_row_data, cal_col_ct_avg, __GETCALVAL("Cal-{type}-{plateID}", "num_points")), __GETRANGE(cal_row_data, cal_col_logct, __GETCALVAL("Cal-{type}-{plateID}", "num_points")))*__SETCELL("Cal-{type}-{plateID}", "rsq", 1)</f>

</xml_diff>

<commit_message>
__UPPER custom function, sites case fix, Excel calculator exception avoidance
</commit_message>
<xml_diff>
--- a/qpcr_analyzer/qpcr_template_ottawa.xlsx
+++ b/qpcr_analyzer/qpcr_template_ottawa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinwellman/Documents/Health/Wastewater/Code/odm-qpcr-analyzer/qpcr_analyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF0A003-3406-7A4D-A38A-C65A4162C7D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCA0C73-DDAD-5947-A0DD-162D8EAD2A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="1" xr2:uid="{9359BC57-A822-3445-B588-7E071C6D13C9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{9359BC57-A822-3445-B588-7E071C6D13C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,19 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="105">
   <si>
     <t>qPCR Data</t>
   </si>
@@ -244,9 +251,6 @@
     <t>Site</t>
   </si>
   <si>
-    <t>{siteID}</t>
-  </si>
-  <si>
     <t>nPMMoV Ct</t>
   </si>
   <si>
@@ -354,6 +358,9 @@
   <si>
     <t>Sample
 Type</t>
+  </si>
+  <si>
+    <t>__UPPER({siteID})</t>
   </si>
 </sst>
 </file>
@@ -923,6 +930,12 @@
     <xf numFmtId="16" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="12" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -955,12 +968,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1385,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A78BE4-03D0-4C45-A8C6-85FB2F5005D2}">
   <dimension ref="A1:BT10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:G3"/>
+    <sheetView tabSelected="1" topLeftCell="BF1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BX5" sqref="BX5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1534,10 +1541,10 @@
         <v>61</v>
       </c>
       <c r="BS1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BT1" t="s">
         <v>102</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:72" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1627,55 +1634,55 @@
         <v>0</v>
       </c>
       <c r="D3" s="41"/>
-      <c r="E3" s="66" t="e">
+      <c r="E3" s="55" t="e">
         <f ca="1">__QAQCHASFAILEDCATEGORY("NTC", "NTC Error! See {qaqc_sheet}", "NTCs Good", "No NTCs")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
       <c r="H3" s="54"/>
-      <c r="I3" s="67" t="e">
+      <c r="I3" s="56" t="e">
         <f ca="1">__QAQCHASFAILEDCATEGORY("EB", "EB Error! See {qaqc_sheet}", "Extraction Blanks Good", "No Extraction Blanks")</f>
         <v>#NAME?</v>
       </c>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
       <c r="L3" s="51"/>
-      <c r="AP3" s="55" t="s">
+      <c r="AP3" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="AQ3" s="56"/>
-      <c r="AR3" s="56"/>
-      <c r="AS3" s="56"/>
-      <c r="AT3" s="56"/>
-      <c r="AU3" s="56"/>
-      <c r="AV3" s="56"/>
-      <c r="AW3" s="56"/>
-      <c r="AX3" s="56"/>
-      <c r="AY3" s="56"/>
-      <c r="AZ3" s="56"/>
-      <c r="BA3" s="57"/>
+      <c r="AQ3" s="58"/>
+      <c r="AR3" s="58"/>
+      <c r="AS3" s="58"/>
+      <c r="AT3" s="58"/>
+      <c r="AU3" s="58"/>
+      <c r="AV3" s="58"/>
+      <c r="AW3" s="58"/>
+      <c r="AX3" s="58"/>
+      <c r="AY3" s="58"/>
+      <c r="AZ3" s="58"/>
+      <c r="BA3" s="59"/>
       <c r="BB3" s="28"/>
       <c r="BC3" s="29"/>
       <c r="BD3" s="30"/>
-      <c r="BE3" s="58" t="s">
+      <c r="BE3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="BF3" s="58"/>
-      <c r="BG3" s="58"/>
-      <c r="BH3" s="58"/>
-      <c r="BI3" s="58"/>
-      <c r="BJ3" s="58"/>
-      <c r="BK3" s="58"/>
-      <c r="BL3" s="58"/>
-      <c r="BM3" s="58"/>
-      <c r="BN3" s="58"/>
-      <c r="BO3" s="58"/>
-      <c r="BP3" s="58"/>
-      <c r="BQ3" s="58"/>
-      <c r="BR3" s="58"/>
-      <c r="BS3" s="58"/>
-      <c r="BT3" s="59"/>
+      <c r="BF3" s="60"/>
+      <c r="BG3" s="60"/>
+      <c r="BH3" s="60"/>
+      <c r="BI3" s="60"/>
+      <c r="BJ3" s="60"/>
+      <c r="BK3" s="60"/>
+      <c r="BL3" s="60"/>
+      <c r="BM3" s="60"/>
+      <c r="BN3" s="60"/>
+      <c r="BO3" s="60"/>
+      <c r="BP3" s="60"/>
+      <c r="BQ3" s="60"/>
+      <c r="BR3" s="60"/>
+      <c r="BS3" s="60"/>
+      <c r="BT3" s="61"/>
     </row>
     <row r="4" spans="1:72" s="5" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
@@ -1694,43 +1701,43 @@
         <v>69</v>
       </c>
       <c r="G4" s="53" t="s">
-        <v>104</v>
-      </c>
-      <c r="H4" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="61"/>
-      <c r="J4" s="62"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="64"/>
       <c r="K4" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="M4" s="60" t="s">
+      <c r="M4" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="61"/>
-      <c r="O4" s="62"/>
+      <c r="N4" s="63"/>
+      <c r="O4" s="64"/>
       <c r="P4" s="8" t="s">
         <v>33</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="60" t="s">
+      <c r="R4" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="S4" s="63"/>
+      <c r="T4" s="64"/>
+      <c r="U4" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="S4" s="61"/>
-      <c r="T4" s="62"/>
-      <c r="U4" s="8" t="s">
+      <c r="V4" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="V4" s="7" t="s">
-        <v>73</v>
-      </c>
       <c r="W4" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="X4" s="7" t="s">
         <v>7</v>
@@ -1750,27 +1757,27 @@
       <c r="AC4" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="AD4" s="63" t="s">
+      <c r="AD4" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="AE4" s="64"/>
-      <c r="AF4" s="65"/>
+      <c r="AE4" s="66"/>
+      <c r="AF4" s="67"/>
       <c r="AG4" s="9" t="s">
         <v>40</v>
       </c>
       <c r="AH4" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AI4" s="63" t="s">
+      <c r="AI4" s="65" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ4" s="66"/>
+      <c r="AK4" s="67"/>
+      <c r="AL4" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AJ4" s="64"/>
-      <c r="AK4" s="65"/>
-      <c r="AL4" s="7" t="s">
+      <c r="AM4" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="AM4" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="AN4" s="6" t="s">
         <v>3</v>
@@ -1778,38 +1785,38 @@
       <c r="AO4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AP4" s="63" t="s">
-        <v>77</v>
-      </c>
-      <c r="AQ4" s="64"/>
-      <c r="AR4" s="65"/>
+      <c r="AP4" s="65" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ4" s="66"/>
+      <c r="AR4" s="67"/>
       <c r="AS4" s="18" t="s">
         <v>10</v>
       </c>
       <c r="AT4" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="AU4" s="63" t="s">
+      <c r="AU4" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="AV4" s="64"/>
-      <c r="AW4" s="65"/>
+      <c r="AV4" s="66"/>
+      <c r="AW4" s="67"/>
       <c r="AX4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="AY4" s="63" t="s">
+      <c r="AY4" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="AZ4" s="64"/>
-      <c r="BA4" s="65"/>
+      <c r="AZ4" s="66"/>
+      <c r="BA4" s="67"/>
       <c r="BB4" s="19" t="s">
         <v>10</v>
       </c>
       <c r="BC4" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="BD4" s="11" t="s">
         <v>78</v>
-      </c>
-      <c r="BD4" s="11" t="s">
-        <v>79</v>
       </c>
       <c r="BE4" s="20" t="s">
         <v>3</v>
@@ -1818,46 +1825,46 @@
         <v>12</v>
       </c>
       <c r="BG4" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BH4" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BI4" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BJ4" s="13" t="s">
         <v>13</v>
       </c>
       <c r="BK4" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="BL4" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="BM4" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="BN4" s="13" t="s">
         <v>14</v>
       </c>
       <c r="BO4" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="BP4" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="BQ4" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="BR4" s="13" t="s">
         <v>15</v>
       </c>
       <c r="BS4" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="BT4" s="14" t="s">
         <v>83</v>
-      </c>
-      <c r="BT4" s="14" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:72" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1874,20 +1881,20 @@
         <v>23</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="G5" s="15" t="e">
         <f ca="1">__QUOTIFY(__GETDATA(D5, "sample_typeShortDescription"))</f>
         <v>#NAME?</v>
       </c>
       <c r="H5" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="J5" s="21" t="s">
         <v>86</v>
-      </c>
-      <c r="J5" s="21" t="s">
-        <v>87</v>
       </c>
       <c r="K5" s="16" t="e">
         <f>AVERAGE(H5:J5)</f>
@@ -1918,65 +1925,65 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R5" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="S5" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="S5" s="16" t="s">
+      <c r="T5" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="T5" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="U5" s="16" t="e">
-        <f>AVERAGE(R5:T5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V5" s="16" t="e">
-        <f t="shared" ref="V5" si="0">STDEV(R5:T5)</f>
-        <v>#DIV/0!</v>
+      <c r="U5" s="16" t="str">
+        <f>IF(COUNT(R5:T5)&gt;0,AVERAGE(R5:T5),"")</f>
+        <v/>
+      </c>
+      <c r="V5" s="16" t="str">
+        <f>IF(COUNT(R5:T5)&gt;0,STDEV(R5:T5),"")</f>
+        <v/>
       </c>
       <c r="W5" s="17" t="e">
         <f ca="1">IF(G5="PS",40,__SELECT("{value_totvol_0||}", """"))</f>
         <v>#NAME?</v>
       </c>
       <c r="X5" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y5" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="Y5" s="17" t="s">
+      <c r="Z5" s="17" t="str">
+        <f>IF(AND(ISNUMBER(Y5),ISNUMBER(X5)),Y5-X5,"")</f>
+        <v/>
+      </c>
+      <c r="AA5" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="Z5" s="17" t="e">
-        <f>IF(AND(Y5&lt;&gt;"",X5&lt;&gt;""),Y5-X5,"")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AA5" s="17" t="s">
+      <c r="AB5" s="17" t="s">
         <v>100</v>
-      </c>
-      <c r="AB5" s="17" t="s">
-        <v>101</v>
       </c>
       <c r="AC5" s="49">
         <f>IF(ISERROR(DATEVALUE(B5)),3,IF(DATEVALUE(B5)&gt;=DATE(2021,6,8),3,1.5))</f>
         <v>3</v>
       </c>
       <c r="AD5" s="17" t="str">
-        <f>IF(M5&lt;&gt;"",(M5/$AC5*100)/$AB5,"")</f>
+        <f>IF(AND(ISNUMBER(M5),ISNUMBER($AB5)),(M5/$AC5*100)/$AB5,"")</f>
         <v/>
       </c>
       <c r="AE5" s="17" t="str">
-        <f>IF(N5&lt;&gt;"",(N5/$AC5*100)/$AB5,"")</f>
+        <f t="shared" ref="AE5:AF5" si="0">IF(AND(ISNUMBER(N5),ISNUMBER($AB5)),(N5/$AC5*100)/$AB5,"")</f>
         <v/>
       </c>
       <c r="AF5" s="17" t="str">
-        <f>IF(O5&lt;&gt;"",(O5/$AC5*100)/$AB5,"")</f>
-        <v/>
-      </c>
-      <c r="AG5" s="17" t="e">
-        <f t="shared" ref="AG5" si="1">AVERAGE(AD5:AF5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AH5" s="17" t="e">
-        <f>STDEV(AD5:AF5)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AG5" s="17" t="str">
+        <f>IF(COUNT(AD5:AF5)&gt;0,AVERAGE(AD5:AF5),"")</f>
+        <v/>
+      </c>
+      <c r="AH5" s="17" t="str">
+        <f>IF(COUNT(AD5:AF5)&gt;0,STDEV(AD5:AF5),"")</f>
+        <v/>
       </c>
       <c r="AI5" s="37" t="str">
         <f>IF(ISNUMBER(R5),10^((R5-__GETCELL(__GETDATA(R5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(R5,"standardCurveID"), "slope", FALSE)),"")</f>
@@ -1990,40 +1997,39 @@
         <f>IF(ISNUMBER(T5),10^((T5-__GETCELL(__GETDATA(T5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(T5,"standardCurveID"), "slope", FALSE)),"")</f>
         <v/>
       </c>
-      <c r="AL5" s="46" t="e">
-        <f t="shared" ref="AL5" si="2">AVERAGE(AI5:AK5)*10</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AM5" s="17" t="e">
-        <f t="shared" ref="AM5" si="3">STDEV(AI5:AK5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AN5" s="35" t="str">
-        <f>C5</f>
-        <v>{sampleDate}</v>
+      <c r="AL5" s="46" t="str">
+        <f>IF(COUNT(AI5:AK5)&gt;0,AVERAGE(AI5:AK5)*10,"")</f>
+        <v/>
+      </c>
+      <c r="AM5" s="17" t="str">
+        <f>IF(COUNT(AI5:AK5)&gt;0,STDEV(AI5:AK5),"")</f>
+        <v/>
+      </c>
+      <c r="AN5" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="AO5" s="15" t="s">
         <v>23</v>
       </c>
       <c r="AP5" s="47" t="str">
-        <f>IF(M5&lt;&gt;"",M5/(AL5),"")</f>
+        <f>IF(AND(ISNUMBER(M5),ISNUMBER($AL5)),M5/($AL5),"")</f>
         <v/>
       </c>
       <c r="AQ5" s="47" t="str">
-        <f>IF(N5&lt;&gt;"",N5/(AL5),"")</f>
+        <f t="shared" ref="AQ5:AR5" si="1">IF(AND(ISNUMBER(N5),ISNUMBER($AL5)),N5/($AL5),"")</f>
         <v/>
       </c>
       <c r="AR5" s="47" t="str">
-        <f>IF(O5&lt;&gt;"",O5/(AL5),"")</f>
-        <v/>
-      </c>
-      <c r="AS5" s="39" t="e">
-        <f t="shared" ref="AS5" si="4">AVERAGE(AP5:AR5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AT5" s="39" t="e">
-        <f t="shared" ref="AT5" si="5">STDEV(AP5:AR5)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AS5" s="39" t="str">
+        <f>IF(COUNT(AP5:AR5)&gt;0,AVERAGE(AP5:AR5),"")</f>
+        <v/>
+      </c>
+      <c r="AT5" s="39" t="str">
+        <f>IF(COUNT(AP5:AR5)&gt;0,STDEV(AP5:AR5),"")</f>
+        <v/>
       </c>
       <c r="AU5" s="31" t="str">
         <f>AD5</f>
@@ -2037,37 +2043,36 @@
         <f>AF5</f>
         <v/>
       </c>
-      <c r="AX5" s="17" t="e">
-        <f t="shared" ref="AX5" si="6">AVERAGE(AU5:AW5)</f>
-        <v>#DIV/0!</v>
+      <c r="AX5" s="17" t="str">
+        <f>IF(COUNT(AU5:AW5)&gt;0,AVERAGE(AU5:AW5),"")</f>
+        <v/>
       </c>
       <c r="AY5" s="31" t="str">
         <f>IF(ISNUMBER(AD5),AD5*$Z5/40*$AA5/$W5*1000,"")</f>
         <v/>
       </c>
       <c r="AZ5" s="31" t="str">
-        <f t="shared" ref="AZ5:BA5" si="7">IF(ISNUMBER(AE5),AE5*$Z5/40*$AA5/$W5*1000,"")</f>
+        <f t="shared" ref="AZ5:BA5" si="2">IF(ISNUMBER(AE5),AE5*$Z5/40*$AA5/$W5*1000,"")</f>
         <v/>
       </c>
       <c r="BA5" s="31" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="BB5" s="17" t="e">
-        <f>AVERAGE(AY5:BA5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BC5" s="32" t="e">
-        <f>(AL5/1.5*100)/$AB5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BD5" s="33" t="e">
-        <f ca="1">BC5*$Z5/40*$AA5/$W5*1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BE5" s="36" t="str">
-        <f>AN5</f>
-        <v>{sampleDate}</v>
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="BB5" s="17" t="str">
+        <f>IF(COUNT(AY5:BA5)&gt;0,AVERAGE(AY5:BA5),"")</f>
+        <v/>
+      </c>
+      <c r="BC5" s="32" t="str">
+        <f>IF(AND(ISNUMBER(AL5),ISNUMBER($AB5)),(AL5/1.5*100)/$AB5,"")</f>
+        <v/>
+      </c>
+      <c r="BD5" s="33" t="str">
+        <f>IF(ISNUMBER(BC5),BC5*$Z5/40*$AA5/$W5*1000,"")</f>
+        <v/>
+      </c>
+      <c r="BE5" s="36" t="s">
+        <v>21</v>
       </c>
       <c r="BF5" s="16" t="str">
         <f>D5</f>
@@ -2085,31 +2090,31 @@
         <f>IF(T5&lt;&gt;"",T5,"")</f>
         <v>{value_npmmov_dil10_2|&lt;ND&gt;|&lt;MISSING&gt;}</v>
       </c>
-      <c r="BJ5" s="16" t="e">
-        <f>AVERAGE(BG5:BI5)</f>
-        <v>#DIV/0!</v>
+      <c r="BJ5" s="16" t="str">
+        <f>IF(COUNT(BG5:BI5)&gt;0,AVERAGE(BG5:BI5),"")</f>
+        <v/>
       </c>
       <c r="BK5" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL5" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="BL5" s="21" t="s">
+      <c r="BM5" s="21" t="s">
         <v>93</v>
-      </c>
-      <c r="BM5" s="21" t="s">
-        <v>94</v>
       </c>
       <c r="BN5" s="16" t="str">
         <f>IF(COUNT(BK5:BM5)&gt;0,AVERAGE(BK5:BM5),"")</f>
         <v/>
       </c>
       <c r="BO5" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="BP5" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="BP5" s="16" t="s">
+      <c r="BQ5" s="16" t="s">
         <v>96</v>
-      </c>
-      <c r="BQ5" s="16" t="s">
-        <v>97</v>
       </c>
       <c r="BR5" s="16" t="str">
         <f>IF(COUNT(BO5:BQ5)&gt;0,AVERAGE(BO5:BQ5),"")</f>
@@ -2197,7 +2202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43405FCF-EE9C-0146-81B2-A2A958472A61}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="103" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -2257,13 +2262,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="D3" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="F3" s="22" t="s">
         <v>86</v>
-      </c>
-      <c r="F3" s="22" t="s">
-        <v>87</v>
       </c>
       <c r="G3" s="22" t="e">
         <f ca="1">AVERAGE(D3:F3)*__SETCELL("Cal-{type}-{plateID}", "avg_std_#",1)</f>

</xml_diff>

<commit_message>
User accounts and reCAPTCHA v3 for website, general fixes to analyzer
</commit_message>
<xml_diff>
--- a/qpcr_analyzer/qpcr_template_ottawa.xlsx
+++ b/qpcr_analyzer/qpcr_template_ottawa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinwellman/Documents/Health/Wastewater/Code/odm-qpcr-analyzer/qpcr_analyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCA0C73-DDAD-5947-A0DD-162D8EAD2A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD9C71D-6362-5842-AF6A-633A61FA1004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{9359BC57-A822-3445-B588-7E071C6D13C9}"/>
   </bookViews>
@@ -1392,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A78BE4-03D0-4C45-A8C6-85FB2F5005D2}">
   <dimension ref="A1:BT10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BF1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BX5" sqref="BX5"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AP5" sqref="AP5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1905,15 +1905,15 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M5" s="38" t="str">
-        <f>IF(ISNUMBER(H5),10^((H5-__GETCELL(__GETDATA(H5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(H5, "standardCurveID"), "slope", FALSE)),"")</f>
+        <f>IF(ISNUMBER(H5),10^((H5-__GETCELL(__GETDATA(H5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(H5, "standardCurveID"), "slope", FALSE)),IF(H5="&lt;ND&gt;",0,""))</f>
         <v/>
       </c>
       <c r="N5" s="38" t="str">
-        <f>IF(ISNUMBER(I5),10^((I5-__GETCELL(__GETDATA(I5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(I5, "standardCurveID"), "slope", FALSE)),"")</f>
+        <f>IF(ISNUMBER(I5),10^((I5-__GETCELL(__GETDATA(I5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(I5, "standardCurveID"), "slope", FALSE)),IF(I5="&lt;ND&gt;",0,""))</f>
         <v/>
       </c>
       <c r="O5" s="38" t="str">
-        <f>IF(ISNUMBER(J5),10^((J5-__GETCELL(__GETDATA(J5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(J5, "standardCurveID"), "slope", FALSE)),"")</f>
+        <f>IF(ISNUMBER(J5),10^((J5-__GETCELL(__GETDATA(J5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(J5, "standardCurveID"), "slope", FALSE)),IF(J5="&lt;ND&gt;",0,""))</f>
         <v/>
       </c>
       <c r="P5" s="16" t="e">
@@ -1986,15 +1986,15 @@
         <v/>
       </c>
       <c r="AI5" s="37" t="str">
-        <f>IF(ISNUMBER(R5),10^((R5-__GETCELL(__GETDATA(R5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(R5,"standardCurveID"), "slope", FALSE)),"")</f>
+        <f>IF(ISNUMBER(R5),10^((R5-__GETCELL(__GETDATA(R5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(R5,"standardCurveID"), "slope", FALSE)),IF(R5="&lt;ND&gt;",0,""))</f>
         <v/>
       </c>
       <c r="AJ5" s="37" t="str">
-        <f>IF(ISNUMBER(S5),10^((S5-__GETCELL(__GETDATA(S5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(S5,"standardCurveID"), "slope", FALSE)),"")</f>
+        <f>IF(ISNUMBER(S5),10^((S5-__GETCELL(__GETDATA(S5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(S5,"standardCurveID"), "slope", FALSE)),IF(S5="&lt;ND&gt;",0,""))</f>
         <v/>
       </c>
       <c r="AK5" s="37" t="str">
-        <f>IF(ISNUMBER(T5),10^((T5-__GETCELL(__GETDATA(T5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(T5,"standardCurveID"), "slope", FALSE)),"")</f>
+        <f>IF(ISNUMBER(T5),10^((T5-__GETCELL(__GETDATA(T5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(T5,"standardCurveID"), "slope", FALSE)),IF(T5="&lt;ND&gt;",0,""))</f>
         <v/>
       </c>
       <c r="AL5" s="46" t="str">

</xml_diff>

<commit_message>
Lambda function runs QPCRUpdater.update only once, at end of execution, instead of twice (at both beginning and end of handler)
</commit_message>
<xml_diff>
--- a/qpcr_analyzer/qpcr_template_ottawa.xlsx
+++ b/qpcr_analyzer/qpcr_template_ottawa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinwellman/Documents/Health/Wastewater/Code/odm-qpcr-analyzer/qpcr_analyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD9C71D-6362-5842-AF6A-633A61FA1004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2102AC80-BEE9-B54C-971F-8FAC2A43DB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{9359BC57-A822-3445-B588-7E071C6D13C9}"/>
   </bookViews>
@@ -770,7 +770,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -904,9 +904,6 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="10" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1392,8 +1389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A78BE4-03D0-4C45-A8C6-85FB2F5005D2}">
   <dimension ref="A1:BT10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AP5" sqref="AP5"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AM5" sqref="AM5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1634,55 +1631,55 @@
         <v>0</v>
       </c>
       <c r="D3" s="41"/>
-      <c r="E3" s="55" t="e">
+      <c r="E3" s="54" t="e">
         <f ca="1">__QAQCHASFAILEDCATEGORY("NTC", "NTC Error! See {qaqc_sheet}", "NTCs Good", "No NTCs")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="56" t="e">
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="55" t="e">
         <f ca="1">__QAQCHASFAILEDCATEGORY("EB", "EB Error! See {qaqc_sheet}", "Extraction Blanks Good", "No Extraction Blanks")</f>
         <v>#NAME?</v>
       </c>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="51"/>
-      <c r="AP3" s="57" t="s">
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="50"/>
+      <c r="AP3" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="AQ3" s="58"/>
-      <c r="AR3" s="58"/>
-      <c r="AS3" s="58"/>
-      <c r="AT3" s="58"/>
-      <c r="AU3" s="58"/>
-      <c r="AV3" s="58"/>
-      <c r="AW3" s="58"/>
-      <c r="AX3" s="58"/>
-      <c r="AY3" s="58"/>
-      <c r="AZ3" s="58"/>
-      <c r="BA3" s="59"/>
+      <c r="AQ3" s="57"/>
+      <c r="AR3" s="57"/>
+      <c r="AS3" s="57"/>
+      <c r="AT3" s="57"/>
+      <c r="AU3" s="57"/>
+      <c r="AV3" s="57"/>
+      <c r="AW3" s="57"/>
+      <c r="AX3" s="57"/>
+      <c r="AY3" s="57"/>
+      <c r="AZ3" s="57"/>
+      <c r="BA3" s="58"/>
       <c r="BB3" s="28"/>
       <c r="BC3" s="29"/>
       <c r="BD3" s="30"/>
-      <c r="BE3" s="60" t="s">
+      <c r="BE3" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="BF3" s="60"/>
-      <c r="BG3" s="60"/>
-      <c r="BH3" s="60"/>
-      <c r="BI3" s="60"/>
-      <c r="BJ3" s="60"/>
-      <c r="BK3" s="60"/>
-      <c r="BL3" s="60"/>
-      <c r="BM3" s="60"/>
-      <c r="BN3" s="60"/>
-      <c r="BO3" s="60"/>
-      <c r="BP3" s="60"/>
-      <c r="BQ3" s="60"/>
-      <c r="BR3" s="60"/>
-      <c r="BS3" s="60"/>
-      <c r="BT3" s="61"/>
+      <c r="BF3" s="59"/>
+      <c r="BG3" s="59"/>
+      <c r="BH3" s="59"/>
+      <c r="BI3" s="59"/>
+      <c r="BJ3" s="59"/>
+      <c r="BK3" s="59"/>
+      <c r="BL3" s="59"/>
+      <c r="BM3" s="59"/>
+      <c r="BN3" s="59"/>
+      <c r="BO3" s="59"/>
+      <c r="BP3" s="59"/>
+      <c r="BQ3" s="59"/>
+      <c r="BR3" s="59"/>
+      <c r="BS3" s="59"/>
+      <c r="BT3" s="60"/>
     </row>
     <row r="4" spans="1:72" s="5" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
@@ -1697,39 +1694,39 @@
       <c r="E4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="50" t="s">
+      <c r="F4" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="53" t="s">
+      <c r="G4" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="H4" s="62" t="s">
+      <c r="H4" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="63"/>
-      <c r="J4" s="64"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="63"/>
       <c r="K4" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="M4" s="62" t="s">
+      <c r="M4" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="63"/>
-      <c r="O4" s="64"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="63"/>
       <c r="P4" s="8" t="s">
         <v>33</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="62" t="s">
+      <c r="R4" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="S4" s="63"/>
-      <c r="T4" s="64"/>
+      <c r="S4" s="62"/>
+      <c r="T4" s="63"/>
       <c r="U4" s="8" t="s">
         <v>71</v>
       </c>
@@ -1754,25 +1751,25 @@
       <c r="AB4" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="AC4" s="48" t="s">
+      <c r="AC4" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="AD4" s="65" t="s">
+      <c r="AD4" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="AE4" s="66"/>
-      <c r="AF4" s="67"/>
+      <c r="AE4" s="65"/>
+      <c r="AF4" s="66"/>
       <c r="AG4" s="9" t="s">
         <v>40</v>
       </c>
       <c r="AH4" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AI4" s="65" t="s">
+      <c r="AI4" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="AJ4" s="66"/>
-      <c r="AK4" s="67"/>
+      <c r="AJ4" s="65"/>
+      <c r="AK4" s="66"/>
       <c r="AL4" s="7" t="s">
         <v>74</v>
       </c>
@@ -1785,30 +1782,30 @@
       <c r="AO4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AP4" s="65" t="s">
+      <c r="AP4" s="64" t="s">
         <v>76</v>
       </c>
-      <c r="AQ4" s="66"/>
-      <c r="AR4" s="67"/>
+      <c r="AQ4" s="65"/>
+      <c r="AR4" s="66"/>
       <c r="AS4" s="18" t="s">
         <v>10</v>
       </c>
       <c r="AT4" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="AU4" s="65" t="s">
+      <c r="AU4" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="AV4" s="66"/>
-      <c r="AW4" s="67"/>
+      <c r="AV4" s="65"/>
+      <c r="AW4" s="66"/>
       <c r="AX4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="AY4" s="65" t="s">
+      <c r="AY4" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="AZ4" s="66"/>
-      <c r="BA4" s="67"/>
+      <c r="AZ4" s="65"/>
+      <c r="BA4" s="66"/>
       <c r="BB4" s="19" t="s">
         <v>10</v>
       </c>
@@ -1905,15 +1902,15 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M5" s="38" t="str">
-        <f>IF(ISNUMBER(H5),10^((H5-__GETCELL(__GETDATA(H5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(H5, "standardCurveID"), "slope", FALSE)),IF(H5="&lt;ND&gt;",0,""))</f>
+        <f>IF(ISNUMBER(H5),10^((H5-__GETCELL(__GETDATA(H5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(H5, "standardCurveID"), "slope", FALSE)),IF(H5="&lt;ND&gt;","",""))</f>
         <v/>
       </c>
       <c r="N5" s="38" t="str">
-        <f>IF(ISNUMBER(I5),10^((I5-__GETCELL(__GETDATA(I5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(I5, "standardCurveID"), "slope", FALSE)),IF(I5="&lt;ND&gt;",0,""))</f>
+        <f>IF(ISNUMBER(I5),10^((I5-__GETCELL(__GETDATA(I5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(I5, "standardCurveID"), "slope", FALSE)),IF(I5="&lt;ND&gt;","",""))</f>
         <v/>
       </c>
       <c r="O5" s="38" t="str">
-        <f>IF(ISNUMBER(J5),10^((J5-__GETCELL(__GETDATA(J5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(J5, "standardCurveID"), "slope", FALSE)),IF(J5="&lt;ND&gt;",0,""))</f>
+        <f>IF(ISNUMBER(J5),10^((J5-__GETCELL(__GETDATA(J5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(J5, "standardCurveID"), "slope", FALSE)),IF(J5="&lt;ND&gt;","",""))</f>
         <v/>
       </c>
       <c r="P5" s="16" t="e">
@@ -1961,7 +1958,7 @@
       <c r="AB5" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="AC5" s="49">
+      <c r="AC5" s="48">
         <f>IF(ISERROR(DATEVALUE(B5)),3,IF(DATEVALUE(B5)&gt;=DATE(2021,6,8),3,1.5))</f>
         <v>3</v>
       </c>
@@ -1986,23 +1983,23 @@
         <v/>
       </c>
       <c r="AI5" s="37" t="str">
-        <f>IF(ISNUMBER(R5),10^((R5-__GETCELL(__GETDATA(R5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(R5,"standardCurveID"), "slope", FALSE)),IF(R5="&lt;ND&gt;",0,""))</f>
+        <f>IF(ISNUMBER(R5),10^((R5-__GETCELL(__GETDATA(R5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(R5,"standardCurveID"), "slope", FALSE)),IF(R5="&lt;ND&gt;","",""))</f>
         <v/>
       </c>
       <c r="AJ5" s="37" t="str">
-        <f>IF(ISNUMBER(S5),10^((S5-__GETCELL(__GETDATA(S5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(S5,"standardCurveID"), "slope", FALSE)),IF(S5="&lt;ND&gt;",0,""))</f>
+        <f>IF(ISNUMBER(S5),10^((S5-__GETCELL(__GETDATA(S5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(S5,"standardCurveID"), "slope", FALSE)),IF(S5="&lt;ND&gt;","",""))</f>
         <v/>
       </c>
       <c r="AK5" s="37" t="str">
-        <f>IF(ISNUMBER(T5),10^((T5-__GETCELL(__GETDATA(T5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(T5,"standardCurveID"), "slope", FALSE)),IF(T5="&lt;ND&gt;",0,""))</f>
-        <v/>
-      </c>
-      <c r="AL5" s="46" t="str">
+        <f>IF(ISNUMBER(T5),10^((T5-__GETCELL(__GETDATA(T5,"standardCurveID"), "intercept", FALSE))/__GETCELL(__GETDATA(T5,"standardCurveID"), "slope", FALSE)),IF(T5="&lt;ND&gt;","",""))</f>
+        <v/>
+      </c>
+      <c r="AL5" s="16" t="str">
         <f>IF(COUNT(AI5:AK5)&gt;0,AVERAGE(AI5:AK5)*10,"")</f>
         <v/>
       </c>
       <c r="AM5" s="17" t="str">
-        <f>IF(COUNT(AI5:AK5)&gt;0,STDEV(AI5:AK5),"")</f>
+        <f>IF(COUNT(AI5:AK5)&gt;0,STDEV(AI5:AK5)*10,"")</f>
         <v/>
       </c>
       <c r="AN5" s="35" t="s">
@@ -2011,15 +2008,15 @@
       <c r="AO5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AP5" s="47" t="str">
+      <c r="AP5" s="46" t="str">
         <f>IF(AND(ISNUMBER(M5),ISNUMBER($AL5)),M5/($AL5),"")</f>
         <v/>
       </c>
-      <c r="AQ5" s="47" t="str">
+      <c r="AQ5" s="46" t="str">
         <f t="shared" ref="AQ5:AR5" si="1">IF(AND(ISNUMBER(N5),ISNUMBER($AL5)),N5/($AL5),"")</f>
         <v/>
       </c>
-      <c r="AR5" s="47" t="str">
+      <c r="AR5" s="46" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -2208,31 +2205,31 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" style="52" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" style="51" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="15.5" customWidth="1"/>
     <col min="7" max="7" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="52" t="s">
+    <row r="1" spans="1:7" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="51" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="51" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="40" t="s">
@@ -2241,17 +2238,17 @@
       <c r="C2" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="68" t="s">
+      <c r="D2" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="69"/>
-      <c r="F2" s="70"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="69"/>
       <c r="G2" s="40" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="51" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="22" t="s">
@@ -2276,7 +2273,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="51" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="42"/>
@@ -2289,7 +2286,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="51" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="43"/>
@@ -2302,7 +2299,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="51" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="43"/>
@@ -2315,7 +2312,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="51" t="s">
         <v>29</v>
       </c>
       <c r="F7" s="23" t="s">
@@ -2327,7 +2324,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="51" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>